<commit_message>
Introduced MSTS Functional layout
</commit_message>
<xml_diff>
--- a/data/Benchmarks/MKS.xlsx
+++ b/data/Benchmarks/MKS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\MSTS_FJSP\data\Benchmarks\YFJS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\MSTS_FJSP\data\Benchmarks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9ADEB7-5FF5-4CBA-8C03-AA595FBDABC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3E6F5A-8E8F-40AB-9336-6E137A1A52BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{87D6751E-06B1-440E-A7B4-B38AD42E9B96}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{87D6751E-06B1-440E-A7B4-B38AD42E9B96}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="125">
   <si>
     <t>Shortest Path</t>
   </si>
@@ -406,13 +406,16 @@
   </si>
   <si>
     <t>[467;615]</t>
+  </si>
+  <si>
+    <t>Least Utilised Machine</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -442,6 +445,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -621,7 +641,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -670,24 +690,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1002,55 +1052,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42C717E4-2E19-4E10-82CD-C66DD0E858F2}">
-  <dimension ref="A1:N54"/>
+  <dimension ref="A1:S54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="S28" sqref="S28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="11" max="12" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="28" t="s">
+      <c r="C3" s="41"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="29"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="28" t="s">
+      <c r="F3" s="41"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="29"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="28" t="s">
+      <c r="I3" s="41"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="L3" s="41"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="30"/>
-      <c r="M3" s="29" t="s">
+      <c r="O3" s="42"/>
+      <c r="P3" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="30"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q3" s="42"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="3" t="s">
         <v>1</v>
@@ -1080,693 +1135,703 @@
         <v>3</v>
       </c>
       <c r="K4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="13" t="s">
+      <c r="P4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="14"/>
       <c r="C5" s="15"/>
       <c r="D5" s="16"/>
-      <c r="E5" s="14">
-        <v>2213</v>
-      </c>
-      <c r="F5" s="15">
-        <v>1455</v>
-      </c>
-      <c r="G5" s="16">
-        <v>1379</v>
-      </c>
-      <c r="H5" s="14">
-        <v>2213</v>
-      </c>
-      <c r="I5" s="15">
-        <v>1455</v>
-      </c>
-      <c r="J5" s="16">
-        <v>1379</v>
-      </c>
-      <c r="K5" s="20">
+      <c r="E5" s="30">
+        <v>2048</v>
+      </c>
+      <c r="F5" s="31">
+        <v>1406</v>
+      </c>
+      <c r="G5" s="32">
+        <v>1335</v>
+      </c>
+      <c r="H5" s="14"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="20">
         <v>773</v>
       </c>
-      <c r="L5" s="21"/>
-      <c r="M5" s="15">
+      <c r="O5" s="21"/>
+      <c r="P5" s="20">
+        <v>1318</v>
+      </c>
+      <c r="Q5" s="21">
         <v>1130</v>
       </c>
-      <c r="N5" s="16">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="15"/>
       <c r="D6" s="16"/>
-      <c r="E6" s="14">
-        <v>2143</v>
-      </c>
-      <c r="F6" s="15">
-        <v>1217</v>
-      </c>
-      <c r="G6" s="16">
-        <v>1144</v>
-      </c>
-      <c r="H6" s="14">
-        <v>2143</v>
-      </c>
-      <c r="I6" s="15">
-        <v>1217</v>
-      </c>
-      <c r="J6" s="16">
-        <v>1144</v>
-      </c>
-      <c r="K6" s="14">
+      <c r="E6" s="30">
+        <v>2023</v>
+      </c>
+      <c r="F6" s="35">
+        <v>1126</v>
+      </c>
+      <c r="G6" s="34">
+        <v>1140</v>
+      </c>
+      <c r="H6" s="14"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="14">
         <v>825</v>
       </c>
-      <c r="L6" s="16"/>
-      <c r="M6" s="15">
+      <c r="O6" s="16"/>
+      <c r="P6" s="14">
+        <v>1243</v>
+      </c>
+      <c r="Q6" s="16">
         <v>1133</v>
       </c>
-      <c r="N6" s="16">
-        <v>1243</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="15"/>
       <c r="D7" s="16"/>
-      <c r="E7" s="14">
-        <v>690</v>
+      <c r="E7" s="30">
+        <v>747</v>
       </c>
       <c r="F7" s="22">
-        <v>429</v>
-      </c>
-      <c r="G7" s="23">
-        <v>413</v>
-      </c>
-      <c r="H7" s="14">
-        <v>690</v>
-      </c>
-      <c r="I7" s="22">
-        <v>429</v>
-      </c>
-      <c r="J7" s="23">
-        <v>413</v>
-      </c>
-      <c r="K7" s="14">
+        <v>454</v>
+      </c>
+      <c r="G7" s="36">
+        <v>422</v>
+      </c>
+      <c r="H7" s="14"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="14">
         <v>347</v>
       </c>
-      <c r="L7" s="16"/>
-      <c r="M7" s="15">
+      <c r="O7" s="16"/>
+      <c r="P7" s="14">
+        <v>439</v>
+      </c>
+      <c r="Q7" s="16">
         <v>575</v>
       </c>
-      <c r="N7" s="16">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="15"/>
       <c r="D8" s="16"/>
-      <c r="E8" s="14">
+      <c r="E8" s="30">
         <v>1055</v>
       </c>
-      <c r="F8" s="22">
-        <v>495</v>
-      </c>
-      <c r="G8" s="23">
-        <v>533</v>
-      </c>
-      <c r="H8" s="14">
-        <v>1055</v>
-      </c>
-      <c r="I8" s="22">
-        <v>495</v>
-      </c>
-      <c r="J8" s="23">
-        <v>533</v>
-      </c>
-      <c r="K8" s="14">
+      <c r="F8" s="35">
+        <v>567</v>
+      </c>
+      <c r="G8" s="32">
+        <v>585</v>
+      </c>
+      <c r="H8" s="14"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="14">
         <v>390</v>
       </c>
-      <c r="L8" s="16"/>
-      <c r="M8" s="15">
+      <c r="O8" s="16"/>
+      <c r="P8" s="14">
+        <v>569</v>
+      </c>
+      <c r="Q8" s="16">
         <v>576</v>
       </c>
-      <c r="N8" s="16">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="14">
-        <v>1207</v>
-      </c>
-      <c r="F9" s="15">
-        <v>1060</v>
-      </c>
-      <c r="G9" s="16">
-        <v>1057</v>
-      </c>
-      <c r="H9" s="14">
-        <v>1207</v>
-      </c>
-      <c r="I9" s="15">
-        <v>1060</v>
-      </c>
-      <c r="J9" s="16">
-        <v>1057</v>
-      </c>
-      <c r="K9" s="14">
+      <c r="E9" s="30">
+        <v>1069</v>
+      </c>
+      <c r="F9" s="31">
+        <v>975</v>
+      </c>
+      <c r="G9" s="32">
+        <v>975</v>
+      </c>
+      <c r="H9" s="14"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="14">
         <v>445</v>
       </c>
-      <c r="L9" s="16"/>
-      <c r="M9" s="15">
+      <c r="O9" s="16"/>
+      <c r="P9" s="14">
+        <v>566</v>
+      </c>
+      <c r="Q9" s="16">
         <v>608</v>
       </c>
-      <c r="N9" s="16">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="14">
-        <v>1141</v>
-      </c>
-      <c r="F10" s="15">
+      <c r="E10" s="30">
+        <v>1151</v>
+      </c>
+      <c r="F10" s="31">
         <v>873</v>
       </c>
-      <c r="G10" s="16">
-        <v>775</v>
-      </c>
-      <c r="H10" s="14">
-        <v>1141</v>
-      </c>
-      <c r="I10" s="15">
-        <v>873</v>
-      </c>
-      <c r="J10" s="16">
-        <v>775</v>
-      </c>
-      <c r="K10" s="14" t="s">
+      <c r="G10" s="32">
+        <v>861</v>
+      </c>
+      <c r="H10" s="14"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="L10" s="16">
+      <c r="O10" s="16">
         <v>446</v>
       </c>
-      <c r="M10" s="15">
+      <c r="P10" s="14">
         <v>633</v>
       </c>
-      <c r="N10" s="16">
+      <c r="Q10" s="16">
         <v>633</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="15"/>
       <c r="D11" s="16"/>
-      <c r="E11" s="14">
-        <v>1149</v>
-      </c>
-      <c r="F11" s="15">
-        <v>835</v>
-      </c>
-      <c r="G11" s="16">
-        <v>835</v>
-      </c>
-      <c r="H11" s="14">
-        <v>1149</v>
-      </c>
-      <c r="I11" s="15">
-        <v>835</v>
-      </c>
-      <c r="J11" s="16">
-        <v>835</v>
-      </c>
-      <c r="K11" s="14">
+      <c r="E11" s="30">
+        <v>982</v>
+      </c>
+      <c r="F11" s="31">
+        <v>1101</v>
+      </c>
+      <c r="G11" s="32">
+        <v>1023</v>
+      </c>
+      <c r="H11" s="14"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="14">
         <v>444</v>
       </c>
-      <c r="L11" s="16"/>
-      <c r="M11" s="15">
+      <c r="O11" s="16"/>
+      <c r="P11" s="14">
         <v>628</v>
       </c>
-      <c r="N11" s="16">
+      <c r="Q11" s="16">
         <v>628</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="15"/>
       <c r="D12" s="16"/>
-      <c r="E12" s="14">
-        <v>1073</v>
-      </c>
-      <c r="F12" s="15">
-        <v>489</v>
-      </c>
-      <c r="G12" s="16">
-        <v>515</v>
-      </c>
-      <c r="H12" s="14">
-        <v>1073</v>
-      </c>
-      <c r="I12" s="15">
-        <v>489</v>
-      </c>
-      <c r="J12" s="16">
-        <v>515</v>
-      </c>
-      <c r="K12" s="14">
+      <c r="E12" s="30">
+        <v>1154</v>
+      </c>
+      <c r="F12" s="37">
+        <v>512</v>
+      </c>
+      <c r="G12" s="32">
+        <v>538</v>
+      </c>
+      <c r="H12" s="14"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="14">
         <v>353</v>
       </c>
-      <c r="L12" s="16"/>
-      <c r="M12" s="15">
+      <c r="O12" s="16"/>
+      <c r="P12" s="14">
+        <v>531</v>
+      </c>
+      <c r="Q12" s="16">
         <v>485</v>
       </c>
-      <c r="N12" s="16">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="S12" s="7"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="15"/>
       <c r="D13" s="16"/>
-      <c r="E13" s="14">
+      <c r="E13" s="30">
         <v>554</v>
       </c>
-      <c r="F13" s="22">
-        <v>376</v>
-      </c>
-      <c r="G13" s="23">
-        <v>376</v>
-      </c>
-      <c r="H13" s="14">
-        <v>554</v>
-      </c>
-      <c r="I13" s="22">
-        <v>376</v>
-      </c>
-      <c r="J13" s="23">
-        <v>376</v>
-      </c>
-      <c r="K13" s="14">
+      <c r="F13" s="35">
+        <v>399</v>
+      </c>
+      <c r="G13" s="36">
+        <v>401</v>
+      </c>
+      <c r="H13" s="14"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="14">
         <v>242</v>
       </c>
-      <c r="L13" s="16"/>
-      <c r="M13" s="15">
+      <c r="O13" s="16"/>
+      <c r="P13" s="14">
+        <v>506</v>
+      </c>
+      <c r="Q13" s="16">
         <v>402</v>
       </c>
-      <c r="N13" s="16">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
       <c r="D14" s="16"/>
-      <c r="E14" s="14">
-        <v>793</v>
-      </c>
-      <c r="F14" s="15">
-        <v>754</v>
-      </c>
-      <c r="G14" s="16">
-        <v>754</v>
-      </c>
-      <c r="H14" s="14">
-        <v>793</v>
-      </c>
-      <c r="I14" s="15">
-        <v>754</v>
-      </c>
-      <c r="J14" s="16">
-        <v>754</v>
-      </c>
-      <c r="K14" s="14">
+      <c r="E14" s="30">
+        <v>880</v>
+      </c>
+      <c r="F14" s="31">
+        <v>712</v>
+      </c>
+      <c r="G14" s="32">
+        <v>897</v>
+      </c>
+      <c r="H14" s="14"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="14">
         <v>399</v>
       </c>
-      <c r="L14" s="16"/>
-      <c r="M14" s="15">
+      <c r="O14" s="16"/>
+      <c r="P14" s="14">
+        <v>541</v>
+      </c>
+      <c r="Q14" s="16">
         <v>513</v>
       </c>
-      <c r="N14" s="16">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="14"/>
       <c r="C15" s="15"/>
       <c r="D15" s="16"/>
-      <c r="E15" s="14">
-        <v>1520</v>
-      </c>
-      <c r="F15" s="15">
-        <v>792</v>
-      </c>
-      <c r="G15" s="23">
-        <v>731</v>
+      <c r="E15" s="30">
+        <v>1549</v>
+      </c>
+      <c r="F15" s="22">
+        <v>742</v>
+      </c>
+      <c r="G15" s="32">
+        <v>783</v>
       </c>
       <c r="H15" s="14"/>
       <c r="I15" s="15"/>
       <c r="J15" s="16"/>
-      <c r="K15" s="14">
+      <c r="K15" s="14"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="14">
         <v>526</v>
       </c>
-      <c r="L15" s="16"/>
-      <c r="M15" s="15">
+      <c r="O15" s="16"/>
+      <c r="P15" s="14">
+        <v>740</v>
+      </c>
+      <c r="Q15" s="16">
         <v>745</v>
       </c>
-      <c r="N15" s="16">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="14"/>
       <c r="C16" s="15"/>
       <c r="D16" s="16"/>
-      <c r="E16" s="14">
-        <v>1491</v>
-      </c>
-      <c r="F16" s="15">
-        <v>935</v>
-      </c>
-      <c r="G16" s="16">
-        <v>935</v>
+      <c r="E16" s="30">
+        <v>1332</v>
+      </c>
+      <c r="F16" s="31">
+        <v>946</v>
+      </c>
+      <c r="G16" s="32">
+        <v>886</v>
       </c>
       <c r="H16" s="14"/>
       <c r="I16" s="15"/>
       <c r="J16" s="16"/>
-      <c r="K16" s="14">
+      <c r="K16" s="14"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="14">
         <v>512</v>
       </c>
-      <c r="L16" s="16"/>
-      <c r="M16" s="15">
+      <c r="O16" s="16"/>
+      <c r="P16" s="14">
+        <v>813</v>
+      </c>
+      <c r="Q16" s="16">
         <v>744</v>
       </c>
-      <c r="N16" s="16">
-        <v>813</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
       <c r="D17" s="16"/>
-      <c r="E17" s="14">
-        <v>1183</v>
-      </c>
-      <c r="F17" s="15">
-        <v>708</v>
-      </c>
-      <c r="G17" s="16">
-        <v>659</v>
+      <c r="E17" s="30">
+        <v>1227</v>
+      </c>
+      <c r="F17" s="31">
+        <v>727</v>
+      </c>
+      <c r="G17" s="34">
+        <v>706</v>
       </c>
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
       <c r="J17" s="16"/>
-      <c r="K17" s="14">
+      <c r="K17" s="14"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="14">
         <v>405</v>
       </c>
-      <c r="L17" s="16"/>
-      <c r="M17" s="15">
+      <c r="O17" s="16"/>
+      <c r="P17" s="14">
+        <v>717</v>
+      </c>
+      <c r="Q17" s="16">
         <v>553</v>
       </c>
-      <c r="N17" s="16">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="14"/>
       <c r="C18" s="15"/>
       <c r="D18" s="16"/>
-      <c r="E18" s="14">
-        <v>4965</v>
-      </c>
-      <c r="F18" s="15">
-        <v>3364</v>
-      </c>
-      <c r="G18" s="16">
-        <v>1781</v>
+      <c r="E18" s="30">
+        <v>4810</v>
+      </c>
+      <c r="F18" s="31">
+        <v>3282</v>
+      </c>
+      <c r="G18" s="34">
+        <v>1918</v>
       </c>
       <c r="H18" s="14"/>
       <c r="I18" s="15"/>
       <c r="J18" s="16"/>
-      <c r="K18" s="14">
+      <c r="K18" s="14"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="14">
         <v>1317</v>
       </c>
-      <c r="L18" s="16"/>
-      <c r="M18" s="15">
+      <c r="O18" s="16"/>
+      <c r="P18" s="14">
+        <v>2055</v>
+      </c>
+      <c r="Q18" s="16">
         <v>1555</v>
       </c>
-      <c r="N18" s="16">
-        <v>2055</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
       <c r="D19" s="16"/>
-      <c r="E19" s="14">
-        <v>5038</v>
-      </c>
-      <c r="F19" s="15">
-        <v>3926</v>
-      </c>
-      <c r="G19" s="16">
-        <v>1915</v>
+      <c r="E19" s="30">
+        <v>5232</v>
+      </c>
+      <c r="F19" s="31">
+        <v>3849</v>
+      </c>
+      <c r="G19" s="34">
+        <v>2170</v>
       </c>
       <c r="H19" s="14"/>
       <c r="I19" s="15"/>
       <c r="J19" s="16"/>
-      <c r="K19" s="14" t="s">
+      <c r="K19" s="14"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="L19" s="16" t="s">
+      <c r="O19" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="M19" s="15">
+      <c r="P19" s="14">
+        <v>2296</v>
+      </c>
+      <c r="Q19" s="16">
         <v>1690</v>
       </c>
-      <c r="N19" s="16">
-        <v>2296</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B20" s="14"/>
       <c r="C20" s="15"/>
       <c r="D20" s="16"/>
-      <c r="E20" s="14">
-        <v>4988</v>
-      </c>
-      <c r="F20" s="15">
-        <v>3447</v>
-      </c>
-      <c r="G20" s="23">
-        <v>1685</v>
+      <c r="E20" s="30">
+        <v>5284</v>
+      </c>
+      <c r="F20" s="31">
+        <v>3053</v>
+      </c>
+      <c r="G20" s="36">
+        <v>1749</v>
       </c>
       <c r="H20" s="14"/>
       <c r="I20" s="15"/>
       <c r="J20" s="16"/>
-      <c r="K20" s="14" t="s">
+      <c r="K20" s="14"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="L20" s="16" t="s">
+      <c r="O20" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="M20" s="15">
+      <c r="P20" s="14">
+        <v>2006</v>
+      </c>
+      <c r="Q20" s="16">
         <v>1769</v>
       </c>
-      <c r="N20" s="16">
-        <v>2006</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B21" s="14"/>
       <c r="C21" s="15"/>
       <c r="D21" s="16"/>
-      <c r="E21" s="14">
-        <v>5915</v>
-      </c>
-      <c r="F21" s="15">
-        <v>2740</v>
-      </c>
-      <c r="G21" s="23">
-        <v>1634</v>
+      <c r="E21" s="30">
+        <v>6039</v>
+      </c>
+      <c r="F21" s="31">
+        <v>2584</v>
+      </c>
+      <c r="G21" s="36">
+        <v>1598</v>
       </c>
       <c r="H21" s="14"/>
       <c r="I21" s="15"/>
       <c r="J21" s="16"/>
-      <c r="K21" s="14" t="s">
+      <c r="K21" s="14"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="L21" s="16" t="s">
+      <c r="O21" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="M21" s="15">
+      <c r="P21" s="14">
+        <v>2408</v>
+      </c>
+      <c r="Q21" s="16">
         <v>1734</v>
       </c>
-      <c r="N21" s="16">
-        <v>2408</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B22" s="14"/>
       <c r="C22" s="15"/>
       <c r="D22" s="16"/>
-      <c r="E22" s="14">
-        <v>6061</v>
-      </c>
-      <c r="F22" s="15">
-        <v>3091</v>
-      </c>
-      <c r="G22" s="16">
-        <v>1859</v>
+      <c r="E22" s="30">
+        <v>6214</v>
+      </c>
+      <c r="F22" s="31">
+        <v>3849</v>
+      </c>
+      <c r="G22" s="34">
+        <v>1873</v>
       </c>
       <c r="H22" s="14"/>
       <c r="I22" s="15"/>
       <c r="J22" s="16"/>
-      <c r="K22" s="14" t="s">
+      <c r="K22" s="14"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="L22" s="16" t="s">
+      <c r="O22" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="M22" s="15">
+      <c r="P22" s="14">
+        <v>2082</v>
+      </c>
+      <c r="Q22" s="16">
         <v>1735</v>
       </c>
-      <c r="N22" s="16">
-        <v>2082</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
       <c r="D23" s="16"/>
-      <c r="E23" s="14">
-        <v>5808</v>
-      </c>
-      <c r="F23" s="15">
-        <v>3045</v>
-      </c>
-      <c r="G23" s="16">
-        <v>2086</v>
+      <c r="E23" s="30">
+        <v>6206</v>
+      </c>
+      <c r="F23" s="31">
+        <v>2976</v>
+      </c>
+      <c r="G23" s="34">
+        <v>1936</v>
       </c>
       <c r="H23" s="14"/>
       <c r="I23" s="15"/>
       <c r="J23" s="16"/>
-      <c r="K23" s="14" t="s">
+      <c r="K23" s="14"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="L23" s="16" t="s">
+      <c r="O23" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="M23" s="15">
+      <c r="P23" s="14">
+        <v>2038</v>
+      </c>
+      <c r="Q23" s="16">
         <v>1604</v>
       </c>
-      <c r="N23" s="16">
-        <v>2038</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B24" s="17"/>
       <c r="C24" s="18"/>
       <c r="D24" s="19"/>
-      <c r="E24" s="17">
-        <v>5989</v>
-      </c>
-      <c r="F24" s="18">
-        <v>1993</v>
-      </c>
-      <c r="G24" s="19">
-        <v>1741</v>
+      <c r="E24" s="33">
+        <v>6198</v>
+      </c>
+      <c r="F24" s="38">
+        <v>1905</v>
+      </c>
+      <c r="G24" s="39">
+        <v>1688</v>
       </c>
       <c r="H24" s="17"/>
       <c r="I24" s="18"/>
       <c r="J24" s="19"/>
-      <c r="K24" s="17" t="s">
+      <c r="K24" s="17"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="L24" s="19" t="s">
+      <c r="O24" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="M24" s="18">
+      <c r="P24" s="17">
+        <v>2369</v>
+      </c>
+      <c r="Q24" s="19">
         <v>1700</v>
       </c>
-      <c r="N24" s="19">
-        <v>2369</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="27" t="s">
         <v>44</v>
       </c>
@@ -1774,29 +1839,32 @@
       <c r="C25" s="25"/>
       <c r="D25" s="26"/>
       <c r="E25" s="24">
-        <v>653</v>
+        <v>633</v>
       </c>
       <c r="F25" s="25">
-        <v>574</v>
+        <v>510</v>
       </c>
       <c r="G25" s="26">
-        <v>615</v>
+        <v>580</v>
       </c>
       <c r="H25" s="24"/>
       <c r="I25" s="25"/>
       <c r="J25" s="26"/>
-      <c r="K25" s="24">
+      <c r="K25" s="24"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="24">
         <v>257</v>
       </c>
-      <c r="L25" s="26"/>
-      <c r="M25" s="25">
+      <c r="O25" s="26"/>
+      <c r="P25" s="24">
+        <v>327</v>
+      </c>
+      <c r="Q25" s="26">
         <v>321</v>
       </c>
-      <c r="N25" s="26">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="27" t="s">
         <v>45</v>
       </c>
@@ -1804,29 +1872,32 @@
       <c r="C26" s="7"/>
       <c r="D26" s="8"/>
       <c r="E26" s="11">
-        <v>536</v>
+        <v>522</v>
       </c>
       <c r="F26" s="7">
-        <v>452</v>
+        <v>475</v>
       </c>
       <c r="G26" s="8">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="H26" s="11"/>
       <c r="I26" s="7"/>
       <c r="J26" s="8"/>
-      <c r="K26" s="11">
+      <c r="K26" s="11"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="11">
         <v>289</v>
       </c>
-      <c r="L26" s="8"/>
-      <c r="M26" s="33">
+      <c r="O26" s="8"/>
+      <c r="P26" s="11">
+        <v>382</v>
+      </c>
+      <c r="Q26" s="45">
         <v>350</v>
       </c>
-      <c r="N26" s="8">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="27" t="s">
         <v>46</v>
       </c>
@@ -1836,27 +1907,30 @@
       <c r="E27" s="11">
         <v>1273</v>
       </c>
-      <c r="F27" s="34">
-        <v>607</v>
+      <c r="F27" s="40">
+        <v>657</v>
       </c>
       <c r="G27" s="8">
-        <v>876</v>
+        <v>813</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="7"/>
       <c r="J27" s="8"/>
-      <c r="K27" s="11">
+      <c r="K27" s="11"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="11">
         <v>576</v>
       </c>
-      <c r="L27" s="8"/>
-      <c r="M27" s="33">
+      <c r="O27" s="8"/>
+      <c r="P27" s="11">
+        <v>710</v>
+      </c>
+      <c r="Q27" s="45">
         <v>631</v>
       </c>
-      <c r="N27" s="8">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="27" t="s">
         <v>47</v>
       </c>
@@ -1864,29 +1938,32 @@
       <c r="C28" s="7"/>
       <c r="D28" s="8"/>
       <c r="E28" s="11">
-        <v>1328</v>
-      </c>
-      <c r="F28" s="32">
-        <v>702</v>
+        <v>1388</v>
+      </c>
+      <c r="F28" s="28">
+        <v>744</v>
       </c>
       <c r="G28" s="8">
-        <v>702</v>
+        <v>909</v>
       </c>
       <c r="H28" s="11"/>
       <c r="I28" s="7"/>
       <c r="J28" s="8"/>
-      <c r="K28" s="11">
+      <c r="K28" s="11"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="11">
         <v>606</v>
       </c>
-      <c r="L28" s="8"/>
-      <c r="M28" s="33">
+      <c r="O28" s="8"/>
+      <c r="P28" s="11">
+        <v>653</v>
+      </c>
+      <c r="Q28" s="45">
         <v>607</v>
       </c>
-      <c r="N28" s="8">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="27" t="s">
         <v>48</v>
       </c>
@@ -1894,31 +1971,34 @@
       <c r="C29" s="7"/>
       <c r="D29" s="8"/>
       <c r="E29" s="11">
-        <v>921</v>
-      </c>
-      <c r="F29" s="32">
+        <v>1009</v>
+      </c>
+      <c r="F29" s="28">
+        <v>730</v>
+      </c>
+      <c r="G29" s="8">
         <v>644</v>
-      </c>
-      <c r="G29" s="8">
-        <v>673</v>
       </c>
       <c r="H29" s="11"/>
       <c r="I29" s="7"/>
       <c r="J29" s="8"/>
-      <c r="K29" s="11" t="s">
+      <c r="K29" s="11"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="L29" s="8" t="s">
+      <c r="O29" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="M29" s="33">
+      <c r="P29" s="11">
+        <v>482</v>
+      </c>
+      <c r="Q29" s="45">
         <v>505</v>
       </c>
-      <c r="N29" s="8">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="27" t="s">
         <v>49</v>
       </c>
@@ -1926,31 +2006,34 @@
       <c r="C30" s="7"/>
       <c r="D30" s="8"/>
       <c r="E30" s="11">
-        <v>978</v>
-      </c>
-      <c r="F30" s="32">
-        <v>727</v>
+        <v>1181</v>
+      </c>
+      <c r="F30" s="28">
+        <v>648</v>
       </c>
       <c r="G30" s="8">
-        <v>628</v>
+        <v>649</v>
       </c>
       <c r="H30" s="11"/>
       <c r="I30" s="7"/>
       <c r="J30" s="8"/>
-      <c r="K30" s="11" t="s">
+      <c r="K30" s="11"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="L30" s="8" t="s">
+      <c r="O30" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="M30" s="33">
+      <c r="P30" s="11">
+        <v>489</v>
+      </c>
+      <c r="Q30" s="45">
         <v>497</v>
       </c>
-      <c r="N30" s="8">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="27" t="s">
         <v>50</v>
       </c>
@@ -1958,31 +2041,34 @@
       <c r="C31" s="7"/>
       <c r="D31" s="8"/>
       <c r="E31" s="11">
-        <v>2144</v>
-      </c>
-      <c r="F31" s="32">
+        <v>2140</v>
+      </c>
+      <c r="F31" s="28">
+        <v>1302</v>
+      </c>
+      <c r="G31" s="8">
         <v>1315</v>
-      </c>
-      <c r="G31" s="8">
-        <v>1347</v>
       </c>
       <c r="H31" s="11"/>
       <c r="I31" s="7"/>
       <c r="J31" s="8"/>
-      <c r="K31" s="11" t="s">
+      <c r="K31" s="11"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="L31" s="8" t="s">
+      <c r="O31" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="M31" s="33">
+      <c r="P31" s="11">
+        <v>717</v>
+      </c>
+      <c r="Q31" s="45">
         <v>632</v>
       </c>
-      <c r="N31" s="8">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="27" t="s">
         <v>51</v>
       </c>
@@ -1990,31 +2076,34 @@
       <c r="C32" s="7"/>
       <c r="D32" s="8"/>
       <c r="E32" s="11">
-        <v>1532</v>
-      </c>
-      <c r="F32" s="32">
-        <v>1376</v>
+        <v>1697</v>
+      </c>
+      <c r="F32" s="28">
+        <v>1475</v>
       </c>
       <c r="G32" s="8">
-        <v>1500</v>
+        <v>1397</v>
       </c>
       <c r="H32" s="11"/>
       <c r="I32" s="7"/>
       <c r="J32" s="8"/>
-      <c r="K32" s="11" t="s">
+      <c r="K32" s="11"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="L32" s="8" t="s">
+      <c r="O32" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="M32" s="33">
+      <c r="P32" s="11">
+        <v>847</v>
+      </c>
+      <c r="Q32" s="45">
         <v>706</v>
       </c>
-      <c r="N32" s="8">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="27" t="s">
         <v>52</v>
       </c>
@@ -2022,9 +2111,9 @@
       <c r="C33" s="7"/>
       <c r="D33" s="8"/>
       <c r="E33" s="11">
-        <v>892</v>
-      </c>
-      <c r="F33" s="32">
+        <v>977</v>
+      </c>
+      <c r="F33" s="28">
         <v>819</v>
       </c>
       <c r="G33" s="8">
@@ -2033,20 +2122,23 @@
       <c r="H33" s="11"/>
       <c r="I33" s="7"/>
       <c r="J33" s="8"/>
-      <c r="K33" s="11" t="s">
+      <c r="K33" s="11"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="L33" s="8" t="s">
+      <c r="O33" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="M33" s="33">
+      <c r="P33" s="11">
+        <v>535</v>
+      </c>
+      <c r="Q33" s="45">
         <v>533</v>
       </c>
-      <c r="N33" s="8">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="27" t="s">
         <v>53</v>
       </c>
@@ -2054,31 +2146,34 @@
       <c r="C34" s="7"/>
       <c r="D34" s="8"/>
       <c r="E34" s="11">
-        <v>1280</v>
-      </c>
-      <c r="F34" s="32">
-        <v>1007</v>
+        <v>1082</v>
+      </c>
+      <c r="F34" s="28">
+        <v>959</v>
       </c>
       <c r="G34" s="8">
-        <v>833</v>
+        <v>740</v>
       </c>
       <c r="H34" s="11"/>
       <c r="I34" s="7"/>
       <c r="J34" s="8"/>
-      <c r="K34" s="11" t="s">
+      <c r="K34" s="11"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="L34" s="8" t="s">
+      <c r="O34" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="M34" s="33">
+      <c r="P34" s="11">
+        <v>629</v>
+      </c>
+      <c r="Q34" s="45">
         <v>621</v>
       </c>
-      <c r="N34" s="8">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="27" t="s">
         <v>54</v>
       </c>
@@ -2086,31 +2181,34 @@
       <c r="C35" s="7"/>
       <c r="D35" s="8"/>
       <c r="E35" s="11">
-        <v>2440</v>
-      </c>
-      <c r="F35" s="32">
-        <v>1308</v>
+        <v>2653</v>
+      </c>
+      <c r="F35" s="28">
+        <v>1258</v>
       </c>
       <c r="G35" s="8">
-        <v>1221</v>
+        <v>1153</v>
       </c>
       <c r="H35" s="11"/>
       <c r="I35" s="7"/>
       <c r="J35" s="8"/>
-      <c r="K35" s="11" t="s">
+      <c r="K35" s="11"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="L35" s="8" t="s">
+      <c r="O35" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="M35" s="33">
+      <c r="P35" s="11">
+        <v>708</v>
+      </c>
+      <c r="Q35" s="45">
         <v>767</v>
       </c>
-      <c r="N35" s="8">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="27" t="s">
         <v>55</v>
       </c>
@@ -2118,31 +2216,34 @@
       <c r="C36" s="7"/>
       <c r="D36" s="8"/>
       <c r="E36" s="11">
-        <v>1886</v>
-      </c>
-      <c r="F36" s="32">
-        <v>1502</v>
+        <v>2016</v>
+      </c>
+      <c r="F36" s="28">
+        <v>1511</v>
       </c>
       <c r="G36" s="8">
-        <v>1336</v>
+        <v>1357</v>
       </c>
       <c r="H36" s="11"/>
       <c r="I36" s="7"/>
       <c r="J36" s="8"/>
-      <c r="K36" s="11" t="s">
+      <c r="K36" s="11"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="L36" s="8" t="s">
+      <c r="O36" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="M36" s="33">
+      <c r="P36" s="11">
+        <v>720</v>
+      </c>
+      <c r="Q36" s="45">
         <v>727</v>
       </c>
-      <c r="N36" s="8">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="27" t="s">
         <v>56</v>
       </c>
@@ -2150,31 +2251,34 @@
       <c r="C37" s="7"/>
       <c r="D37" s="8"/>
       <c r="E37" s="11">
-        <v>1298</v>
-      </c>
-      <c r="F37" s="32">
-        <v>926</v>
-      </c>
-      <c r="G37" s="35">
-        <v>759</v>
+        <v>1401</v>
+      </c>
+      <c r="F37" s="28">
+        <v>860</v>
+      </c>
+      <c r="G37" s="29">
+        <v>946</v>
       </c>
       <c r="H37" s="11"/>
       <c r="I37" s="7"/>
       <c r="J37" s="8"/>
-      <c r="K37" s="11" t="s">
+      <c r="K37" s="11"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="L37" s="8" t="s">
+      <c r="O37" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="M37" s="33">
+      <c r="P37" s="11">
+        <v>766</v>
+      </c>
+      <c r="Q37" s="45">
         <v>768</v>
       </c>
-      <c r="N37" s="8">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="27" t="s">
         <v>57</v>
       </c>
@@ -2182,31 +2286,34 @@
       <c r="C38" s="7"/>
       <c r="D38" s="8"/>
       <c r="E38" s="11">
-        <v>2072</v>
-      </c>
-      <c r="F38" s="32">
-        <v>1245</v>
+        <v>1796</v>
+      </c>
+      <c r="F38" s="28">
+        <v>1003</v>
       </c>
       <c r="G38" s="8">
-        <v>985</v>
+        <v>1030</v>
       </c>
       <c r="H38" s="11"/>
       <c r="I38" s="7"/>
       <c r="J38" s="8"/>
-      <c r="K38" s="11" t="s">
+      <c r="K38" s="11"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="L38" s="8" t="s">
+      <c r="O38" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="M38" s="33">
+      <c r="P38" s="11">
+        <v>871</v>
+      </c>
+      <c r="Q38" s="45">
         <v>888</v>
       </c>
-      <c r="N38" s="8">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="27" t="s">
         <v>58</v>
       </c>
@@ -2214,31 +2321,34 @@
       <c r="C39" s="7"/>
       <c r="D39" s="8"/>
       <c r="E39" s="11">
-        <v>2671</v>
-      </c>
-      <c r="F39" s="32">
-        <v>1219</v>
+        <v>2457</v>
+      </c>
+      <c r="F39" s="28">
+        <v>1315</v>
       </c>
       <c r="G39" s="8">
-        <v>1327</v>
+        <v>1281</v>
       </c>
       <c r="H39" s="11"/>
       <c r="I39" s="7"/>
       <c r="J39" s="8"/>
-      <c r="K39" s="11" t="s">
+      <c r="K39" s="11"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="L39" s="8" t="s">
+      <c r="O39" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="M39" s="33">
+      <c r="P39" s="11">
+        <v>818</v>
+      </c>
+      <c r="Q39" s="45">
         <v>788</v>
       </c>
-      <c r="N39" s="8">
-        <v>818</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="27" t="s">
         <v>59</v>
       </c>
@@ -2246,31 +2356,34 @@
       <c r="C40" s="7"/>
       <c r="D40" s="8"/>
       <c r="E40" s="11">
-        <v>2534</v>
-      </c>
-      <c r="F40" s="32">
-        <v>1746</v>
+        <v>2547</v>
+      </c>
+      <c r="F40" s="28">
+        <v>1535</v>
       </c>
       <c r="G40" s="8">
-        <v>1725</v>
+        <v>1953</v>
       </c>
       <c r="H40" s="11"/>
       <c r="I40" s="7"/>
       <c r="J40" s="8"/>
-      <c r="K40" s="11" t="s">
+      <c r="K40" s="11"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="L40" s="8" t="s">
+      <c r="O40" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="M40" s="33">
+      <c r="P40" s="11">
+        <v>831</v>
+      </c>
+      <c r="Q40" s="45">
         <v>808</v>
       </c>
-      <c r="N40" s="8">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="27" t="s">
         <v>60</v>
       </c>
@@ -2278,31 +2391,34 @@
       <c r="C41" s="7"/>
       <c r="D41" s="8"/>
       <c r="E41" s="11">
-        <v>1560</v>
-      </c>
-      <c r="F41" s="32">
-        <v>1402</v>
+        <v>1449</v>
+      </c>
+      <c r="F41" s="28">
+        <v>1168</v>
       </c>
       <c r="G41" s="8">
-        <v>1319</v>
+        <v>1222</v>
       </c>
       <c r="H41" s="11"/>
       <c r="I41" s="7"/>
       <c r="J41" s="8"/>
-      <c r="K41" s="11" t="s">
+      <c r="K41" s="11"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="L41" s="8" t="s">
+      <c r="O41" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="M41" s="33">
+      <c r="P41" s="11">
+        <v>910</v>
+      </c>
+      <c r="Q41" s="45">
         <v>935</v>
       </c>
-      <c r="N41" s="8">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="27" t="s">
         <v>61</v>
       </c>
@@ -2310,31 +2426,34 @@
       <c r="C42" s="7"/>
       <c r="D42" s="8"/>
       <c r="E42" s="11">
-        <v>2027</v>
-      </c>
-      <c r="F42" s="32">
-        <v>1122</v>
+        <v>2089</v>
+      </c>
+      <c r="F42" s="28">
+        <v>1312</v>
       </c>
       <c r="G42" s="8">
-        <v>1192</v>
+        <v>1172</v>
       </c>
       <c r="H42" s="11"/>
       <c r="I42" s="7"/>
       <c r="J42" s="8"/>
-      <c r="K42" s="11" t="s">
+      <c r="K42" s="11"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="L42" s="8" t="s">
+      <c r="O42" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="M42" s="33">
+      <c r="P42" s="11">
+        <v>951</v>
+      </c>
+      <c r="Q42" s="45">
         <v>939</v>
       </c>
-      <c r="N42" s="8">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="27" t="s">
         <v>62</v>
       </c>
@@ -2342,31 +2461,34 @@
       <c r="C43" s="7"/>
       <c r="D43" s="8"/>
       <c r="E43" s="11">
-        <v>1434</v>
-      </c>
-      <c r="F43" s="32">
-        <v>1147</v>
+        <v>1740</v>
+      </c>
+      <c r="F43" s="28">
+        <v>1040</v>
       </c>
       <c r="G43" s="8">
-        <v>841</v>
+        <v>1011</v>
       </c>
       <c r="H43" s="11"/>
       <c r="I43" s="7"/>
       <c r="J43" s="8"/>
-      <c r="K43" s="11" t="s">
+      <c r="K43" s="11"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="L43" s="8" t="s">
+      <c r="O43" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="M43" s="33">
+      <c r="P43" s="11">
+        <v>601</v>
+      </c>
+      <c r="Q43" s="45">
         <v>598</v>
       </c>
-      <c r="N43" s="8">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="27" t="s">
         <v>63</v>
       </c>
@@ -2374,31 +2496,34 @@
       <c r="C44" s="7"/>
       <c r="D44" s="8"/>
       <c r="E44" s="11">
-        <v>2381</v>
-      </c>
-      <c r="F44" s="32">
-        <v>1248</v>
+        <v>2345</v>
+      </c>
+      <c r="F44" s="28">
+        <v>1315</v>
       </c>
       <c r="G44" s="8">
-        <v>1206</v>
+        <v>1309</v>
       </c>
       <c r="H44" s="11"/>
       <c r="I44" s="7"/>
       <c r="J44" s="8"/>
-      <c r="K44" s="11" t="s">
+      <c r="K44" s="11"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="L44" s="8" t="s">
+      <c r="O44" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="M44" s="33">
+      <c r="P44" s="11">
+        <v>815</v>
+      </c>
+      <c r="Q44" s="45">
         <v>854</v>
       </c>
-      <c r="N44" s="8">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="27" t="s">
         <v>64</v>
       </c>
@@ -2406,31 +2531,34 @@
       <c r="C45" s="7"/>
       <c r="D45" s="8"/>
       <c r="E45" s="11">
-        <v>1991</v>
-      </c>
-      <c r="F45" s="32">
-        <v>1232</v>
+        <v>1949</v>
+      </c>
+      <c r="F45" s="28">
+        <v>1378</v>
       </c>
       <c r="G45" s="8">
-        <v>1409</v>
+        <v>1365</v>
       </c>
       <c r="H45" s="11"/>
       <c r="I45" s="7"/>
       <c r="J45" s="8"/>
-      <c r="K45" s="11" t="s">
+      <c r="K45" s="11"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="8"/>
+      <c r="N45" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="L45" s="8" t="s">
+      <c r="O45" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="M45" s="33">
+      <c r="P45" s="11">
+        <v>965</v>
+      </c>
+      <c r="Q45" s="45">
         <v>937</v>
       </c>
-      <c r="N45" s="8">
-        <v>965</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="27" t="s">
         <v>65</v>
       </c>
@@ -2438,31 +2566,34 @@
       <c r="C46" s="7"/>
       <c r="D46" s="8"/>
       <c r="E46" s="11">
-        <v>2228</v>
-      </c>
-      <c r="F46" s="32">
-        <v>1375</v>
+        <v>1985</v>
+      </c>
+      <c r="F46" s="28">
+        <v>1603</v>
       </c>
       <c r="G46" s="8">
-        <v>1226</v>
+        <v>1212</v>
       </c>
       <c r="H46" s="11"/>
       <c r="I46" s="7"/>
       <c r="J46" s="8"/>
-      <c r="K46" s="11" t="s">
+      <c r="K46" s="11"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="8"/>
+      <c r="N46" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="L46" s="8" t="s">
+      <c r="O46" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="M46" s="33">
+      <c r="P46" s="11">
+        <v>902</v>
+      </c>
+      <c r="Q46" s="45">
         <v>826</v>
       </c>
-      <c r="N46" s="8">
-        <v>902</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="27" t="s">
         <v>66</v>
       </c>
@@ -2470,31 +2601,34 @@
       <c r="C47" s="7"/>
       <c r="D47" s="8"/>
       <c r="E47" s="11">
-        <v>1450</v>
-      </c>
-      <c r="F47" s="32">
-        <v>1201</v>
+        <v>1429</v>
+      </c>
+      <c r="F47" s="28">
+        <v>1136</v>
       </c>
       <c r="G47" s="8">
-        <v>853</v>
+        <v>902</v>
       </c>
       <c r="H47" s="11"/>
       <c r="I47" s="7"/>
       <c r="J47" s="8"/>
-      <c r="K47" s="11" t="s">
+      <c r="K47" s="11"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="8"/>
+      <c r="N47" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="L47" s="8" t="s">
+      <c r="O47" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="M47" s="33">
+      <c r="P47" s="11">
+        <v>632</v>
+      </c>
+      <c r="Q47" s="45">
         <v>548</v>
       </c>
-      <c r="N47" s="8">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="27" t="s">
         <v>67</v>
       </c>
@@ -2502,31 +2636,34 @@
       <c r="C48" s="7"/>
       <c r="D48" s="8"/>
       <c r="E48" s="11">
-        <v>1604</v>
-      </c>
-      <c r="F48" s="32">
-        <v>1110</v>
+        <v>1847</v>
+      </c>
+      <c r="F48" s="28">
+        <v>1014</v>
       </c>
       <c r="G48" s="8">
-        <v>969</v>
+        <v>1037</v>
       </c>
       <c r="H48" s="11"/>
       <c r="I48" s="7"/>
       <c r="J48" s="8"/>
-      <c r="K48" s="11" t="s">
+      <c r="K48" s="11"/>
+      <c r="L48" s="7"/>
+      <c r="M48" s="8"/>
+      <c r="N48" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="L48" s="8" t="s">
+      <c r="O48" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="M48" s="33">
+      <c r="P48" s="11">
+        <v>674</v>
+      </c>
+      <c r="Q48" s="45">
         <v>687</v>
       </c>
-      <c r="N48" s="8">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="27" t="s">
         <v>68</v>
       </c>
@@ -2534,31 +2671,34 @@
       <c r="C49" s="7"/>
       <c r="D49" s="8"/>
       <c r="E49" s="11">
-        <v>2869</v>
-      </c>
-      <c r="F49" s="32">
-        <v>1163</v>
+        <v>3083</v>
+      </c>
+      <c r="F49" s="28">
+        <v>1201</v>
       </c>
       <c r="G49" s="8">
-        <v>1176</v>
+        <v>1124</v>
       </c>
       <c r="H49" s="11"/>
       <c r="I49" s="7"/>
       <c r="J49" s="8"/>
-      <c r="K49" s="11" t="s">
+      <c r="K49" s="11"/>
+      <c r="L49" s="7"/>
+      <c r="M49" s="8"/>
+      <c r="N49" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="L49" s="8" t="s">
+      <c r="O49" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="M49" s="33">
+      <c r="P49" s="11">
+        <v>897</v>
+      </c>
+      <c r="Q49" s="45">
         <v>885</v>
       </c>
-      <c r="N49" s="8">
-        <v>897</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="27" t="s">
         <v>69</v>
       </c>
@@ -2566,31 +2706,34 @@
       <c r="C50" s="7"/>
       <c r="D50" s="8"/>
       <c r="E50" s="11">
-        <v>2767</v>
-      </c>
-      <c r="F50" s="32">
-        <v>1445</v>
+        <v>2339</v>
+      </c>
+      <c r="F50" s="28">
+        <v>1301</v>
       </c>
       <c r="G50" s="8">
-        <v>1592</v>
+        <v>1450</v>
       </c>
       <c r="H50" s="11"/>
       <c r="I50" s="7"/>
       <c r="J50" s="8"/>
-      <c r="K50" s="11" t="s">
+      <c r="K50" s="11"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="8"/>
+      <c r="N50" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="L50" s="8" t="s">
+      <c r="O50" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="M50" s="33">
+      <c r="P50" s="11">
+        <v>903</v>
+      </c>
+      <c r="Q50" s="45">
         <v>915</v>
       </c>
-      <c r="N50" s="8">
-        <v>903</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="27" t="s">
         <v>70</v>
       </c>
@@ -2598,31 +2741,34 @@
       <c r="C51" s="7"/>
       <c r="D51" s="8"/>
       <c r="E51" s="11">
-        <v>3049</v>
-      </c>
-      <c r="F51" s="32">
-        <v>1926</v>
+        <v>2991</v>
+      </c>
+      <c r="F51" s="28">
+        <v>1675</v>
       </c>
       <c r="G51" s="8">
-        <v>1626</v>
+        <v>1638</v>
       </c>
       <c r="H51" s="11"/>
       <c r="I51" s="7"/>
       <c r="J51" s="8"/>
-      <c r="K51" s="11" t="s">
+      <c r="K51" s="11"/>
+      <c r="L51" s="7"/>
+      <c r="M51" s="8"/>
+      <c r="N51" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="L51" s="8" t="s">
+      <c r="O51" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="M51" s="33">
+      <c r="P51" s="11">
+        <v>981</v>
+      </c>
+      <c r="Q51" s="45">
         <v>982</v>
       </c>
-      <c r="N51" s="8">
-        <v>981</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="27" t="s">
         <v>71</v>
       </c>
@@ -2630,31 +2776,34 @@
       <c r="C52" s="7"/>
       <c r="D52" s="8"/>
       <c r="E52" s="11">
-        <v>2319</v>
-      </c>
-      <c r="F52" s="32">
-        <v>1272</v>
+        <v>2402</v>
+      </c>
+      <c r="F52" s="28">
+        <v>1567</v>
       </c>
       <c r="G52" s="8">
-        <v>1042</v>
+        <v>1210</v>
       </c>
       <c r="H52" s="11"/>
       <c r="I52" s="7"/>
       <c r="J52" s="8"/>
-      <c r="K52" s="11" t="s">
+      <c r="K52" s="11"/>
+      <c r="L52" s="7"/>
+      <c r="M52" s="8"/>
+      <c r="N52" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="L52" s="8" t="s">
+      <c r="O52" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="M52" s="33">
+      <c r="P52" s="11">
+        <v>703</v>
+      </c>
+      <c r="Q52" s="45">
         <v>633</v>
       </c>
-      <c r="N52" s="8">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="27" t="s">
         <v>72</v>
       </c>
@@ -2662,31 +2811,34 @@
       <c r="C53" s="7"/>
       <c r="D53" s="8"/>
       <c r="E53" s="11">
-        <v>2587</v>
-      </c>
-      <c r="F53" s="32">
-        <v>1692</v>
+        <v>2843</v>
+      </c>
+      <c r="F53" s="28">
+        <v>1993</v>
       </c>
       <c r="G53" s="8">
-        <v>1684</v>
+        <v>1633</v>
       </c>
       <c r="H53" s="11"/>
       <c r="I53" s="7"/>
       <c r="J53" s="8"/>
-      <c r="K53" s="11" t="s">
+      <c r="K53" s="11"/>
+      <c r="L53" s="7"/>
+      <c r="M53" s="8"/>
+      <c r="N53" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="L53" s="8" t="s">
+      <c r="O53" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="M53" s="33">
+      <c r="P53" s="11">
+        <v>760</v>
+      </c>
+      <c r="Q53" s="45">
         <v>800</v>
       </c>
-      <c r="N53" s="8">
-        <v>760</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="27" t="s">
         <v>73</v>
       </c>
@@ -2694,38 +2846,42 @@
       <c r="C54" s="9"/>
       <c r="D54" s="10"/>
       <c r="E54" s="12">
-        <v>2506</v>
+        <v>2637</v>
       </c>
       <c r="F54" s="9">
-        <v>1044</v>
+        <v>1084</v>
       </c>
       <c r="G54" s="10">
-        <v>1077</v>
+        <v>1073</v>
       </c>
       <c r="H54" s="12"/>
       <c r="I54" s="9"/>
       <c r="J54" s="10"/>
-      <c r="K54" s="12" t="s">
+      <c r="K54" s="12"/>
+      <c r="L54" s="9"/>
+      <c r="M54" s="10"/>
+      <c r="N54" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="L54" s="10" t="s">
+      <c r="O54" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="M54" s="9">
+      <c r="P54" s="12">
+        <v>657</v>
+      </c>
+      <c r="Q54" s="10">
         <v>640</v>
       </c>
-      <c r="N54" s="10">
-        <v>657</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="M3:N3"/>
+  <mergeCells count="7">
+    <mergeCell ref="P3:Q3"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="E3:G3"/>
-    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="K3:M3"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Successful implementation of Critical Path OS swap method
</commit_message>
<xml_diff>
--- a/data/Benchmarks/MKS.xlsx
+++ b/data/Benchmarks/MKS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\MSTS_FJSP\data\Benchmarks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3E6F5A-8E8F-40AB-9336-6E137A1A52BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704A1CC9-9812-40E6-9368-C200F085D937}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{87D6751E-06B1-440E-A7B4-B38AD42E9B96}"/>
+    <workbookView xWindow="2856" yWindow="144" windowWidth="17280" windowHeight="9132" xr2:uid="{87D6751E-06B1-440E-A7B4-B38AD42E9B96}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="223">
   <si>
     <t>Shortest Path</t>
   </si>
@@ -409,6 +409,300 @@
   </si>
   <si>
     <t>Least Utilised Machine</t>
+  </si>
+  <si>
+    <t>510/475</t>
+  </si>
+  <si>
+    <t>580/467</t>
+  </si>
+  <si>
+    <t>475/409</t>
+  </si>
+  <si>
+    <t>657/586</t>
+  </si>
+  <si>
+    <t>744/686</t>
+  </si>
+  <si>
+    <t>1201/1069</t>
+  </si>
+  <si>
+    <t>730/644</t>
+  </si>
+  <si>
+    <t>648/531</t>
+  </si>
+  <si>
+    <t>1302/979</t>
+  </si>
+  <si>
+    <t>1475/895</t>
+  </si>
+  <si>
+    <t>819/819</t>
+  </si>
+  <si>
+    <t>959/633</t>
+  </si>
+  <si>
+    <t>1258/862</t>
+  </si>
+  <si>
+    <t>1511/1162</t>
+  </si>
+  <si>
+    <t>860/816</t>
+  </si>
+  <si>
+    <t>1003/936</t>
+  </si>
+  <si>
+    <t>1315/994</t>
+  </si>
+  <si>
+    <t>1535/1275</t>
+  </si>
+  <si>
+    <t>1168/1029</t>
+  </si>
+  <si>
+    <t>1312/1022</t>
+  </si>
+  <si>
+    <t>1040/892</t>
+  </si>
+  <si>
+    <t>1315/905</t>
+  </si>
+  <si>
+    <t>1378/1160</t>
+  </si>
+  <si>
+    <t>1603/1013</t>
+  </si>
+  <si>
+    <t>1136/748</t>
+  </si>
+  <si>
+    <t>1014/884</t>
+  </si>
+  <si>
+    <t>1301/1067</t>
+  </si>
+  <si>
+    <t>1675/1213</t>
+  </si>
+  <si>
+    <t>1567/1034</t>
+  </si>
+  <si>
+    <t>1993/1057</t>
+  </si>
+  <si>
+    <t>1084/830</t>
+  </si>
+  <si>
+    <t>529/409</t>
+  </si>
+  <si>
+    <t>813/734</t>
+  </si>
+  <si>
+    <t>909/707</t>
+  </si>
+  <si>
+    <t>644/644</t>
+  </si>
+  <si>
+    <t>649/531</t>
+  </si>
+  <si>
+    <t>1315/1047</t>
+  </si>
+  <si>
+    <t>1397/967</t>
+  </si>
+  <si>
+    <t>740/693</t>
+  </si>
+  <si>
+    <t>1153/970</t>
+  </si>
+  <si>
+    <t>1357/935</t>
+  </si>
+  <si>
+    <t>946/740</t>
+  </si>
+  <si>
+    <t>1030/936</t>
+  </si>
+  <si>
+    <t>1281/1191</t>
+  </si>
+  <si>
+    <t>1953/1598</t>
+  </si>
+  <si>
+    <t>1222/1190</t>
+  </si>
+  <si>
+    <t>1172/1096</t>
+  </si>
+  <si>
+    <t>1011/757</t>
+  </si>
+  <si>
+    <t>1309/927</t>
+  </si>
+  <si>
+    <t>1365/1240</t>
+  </si>
+  <si>
+    <t>1212/1073</t>
+  </si>
+  <si>
+    <t>902/677</t>
+  </si>
+  <si>
+    <t>1037/953</t>
+  </si>
+  <si>
+    <t>1124/1079</t>
+  </si>
+  <si>
+    <t>1450/1161</t>
+  </si>
+  <si>
+    <t>1638/1550</t>
+  </si>
+  <si>
+    <t>1210/921</t>
+  </si>
+  <si>
+    <t>1633/1207</t>
+  </si>
+  <si>
+    <t>1073/846</t>
+  </si>
+  <si>
+    <t>1335/1335</t>
+  </si>
+  <si>
+    <t>1140/824</t>
+  </si>
+  <si>
+    <t>422/404</t>
+  </si>
+  <si>
+    <t>585/472</t>
+  </si>
+  <si>
+    <t>975/688</t>
+  </si>
+  <si>
+    <t>861/685</t>
+  </si>
+  <si>
+    <t>1023/835</t>
+  </si>
+  <si>
+    <t>538/463</t>
+  </si>
+  <si>
+    <t>401/331</t>
+  </si>
+  <si>
+    <t>897/715</t>
+  </si>
+  <si>
+    <t>783/694</t>
+  </si>
+  <si>
+    <t>886/810</t>
+  </si>
+  <si>
+    <t>706/534</t>
+  </si>
+  <si>
+    <t>1918/1655</t>
+  </si>
+  <si>
+    <t>2170/1559</t>
+  </si>
+  <si>
+    <t>1749/1559</t>
+  </si>
+  <si>
+    <t>1598/1355</t>
+  </si>
+  <si>
+    <t>1873/1587</t>
+  </si>
+  <si>
+    <t>1936/1585</t>
+  </si>
+  <si>
+    <t>1688/1688</t>
+  </si>
+  <si>
+    <t>1406/1297</t>
+  </si>
+  <si>
+    <t>1126/902</t>
+  </si>
+  <si>
+    <t>454/404</t>
+  </si>
+  <si>
+    <t>567/472</t>
+  </si>
+  <si>
+    <t>873/685</t>
+  </si>
+  <si>
+    <t>1101/835</t>
+  </si>
+  <si>
+    <t>512/463</t>
+  </si>
+  <si>
+    <t>399/331</t>
+  </si>
+  <si>
+    <t>712/712</t>
+  </si>
+  <si>
+    <t>742/683</t>
+  </si>
+  <si>
+    <t>946/810</t>
+  </si>
+  <si>
+    <t>727/562</t>
+  </si>
+  <si>
+    <t>3282/1744</t>
+  </si>
+  <si>
+    <t>3053/1522</t>
+  </si>
+  <si>
+    <t>3849/2680</t>
+  </si>
+  <si>
+    <t>2584/2542</t>
+  </si>
+  <si>
+    <t>3849/3462</t>
+  </si>
+  <si>
+    <t>2976/2769</t>
+  </si>
+  <si>
+    <t>1905/1537</t>
   </si>
 </sst>
 </file>
@@ -691,7 +985,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -716,13 +1009,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -735,7 +1029,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1054,12 +1348,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42C717E4-2E19-4E10-82CD-C66DD0E858F2}">
   <dimension ref="A1:S54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="6" max="7" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1085,7 +1380,7 @@
         <v>5</v>
       </c>
       <c r="F3" s="41"/>
-      <c r="G3" s="42"/>
+      <c r="G3" s="41"/>
       <c r="H3" s="43" t="s">
         <v>0</v>
       </c>
@@ -1163,14 +1458,14 @@
       <c r="B5" s="14"/>
       <c r="C5" s="15"/>
       <c r="D5" s="16"/>
-      <c r="E5" s="30">
+      <c r="E5" s="29">
         <v>2048</v>
       </c>
-      <c r="F5" s="31">
-        <v>1406</v>
-      </c>
-      <c r="G5" s="32">
-        <v>1335</v>
+      <c r="F5" s="30" t="s">
+        <v>204</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>184</v>
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="15"/>
@@ -1196,14 +1491,14 @@
       <c r="B6" s="14"/>
       <c r="C6" s="15"/>
       <c r="D6" s="16"/>
-      <c r="E6" s="30">
+      <c r="E6" s="29">
         <v>2023</v>
       </c>
-      <c r="F6" s="35">
-        <v>1126</v>
-      </c>
-      <c r="G6" s="34">
-        <v>1140</v>
+      <c r="F6" s="34" t="s">
+        <v>205</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>185</v>
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="15"/>
@@ -1229,14 +1524,14 @@
       <c r="B7" s="14"/>
       <c r="C7" s="15"/>
       <c r="D7" s="16"/>
-      <c r="E7" s="30">
+      <c r="E7" s="29">
         <v>747</v>
       </c>
-      <c r="F7" s="22">
-        <v>454</v>
-      </c>
-      <c r="G7" s="36">
-        <v>422</v>
+      <c r="F7" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>186</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="22"/>
@@ -1262,14 +1557,14 @@
       <c r="B8" s="14"/>
       <c r="C8" s="15"/>
       <c r="D8" s="16"/>
-      <c r="E8" s="30">
+      <c r="E8" s="29">
         <v>1055</v>
       </c>
-      <c r="F8" s="35">
-        <v>567</v>
-      </c>
-      <c r="G8" s="32">
-        <v>585</v>
+      <c r="F8" s="34" t="s">
+        <v>207</v>
+      </c>
+      <c r="G8" s="35" t="s">
+        <v>187</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="22"/>
@@ -1295,14 +1590,14 @@
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="30">
+      <c r="E9" s="29">
         <v>1069</v>
       </c>
-      <c r="F9" s="31">
-        <v>975</v>
-      </c>
-      <c r="G9" s="32">
-        <v>975</v>
+      <c r="F9" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>188</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="15"/>
@@ -1328,14 +1623,14 @@
       <c r="B10" s="14"/>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="30">
+      <c r="E10" s="29">
         <v>1151</v>
       </c>
-      <c r="F10" s="31">
-        <v>873</v>
-      </c>
-      <c r="G10" s="32">
-        <v>861</v>
+      <c r="F10" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>189</v>
       </c>
       <c r="H10" s="14"/>
       <c r="I10" s="15"/>
@@ -1363,14 +1658,14 @@
       <c r="B11" s="14"/>
       <c r="C11" s="15"/>
       <c r="D11" s="16"/>
-      <c r="E11" s="30">
+      <c r="E11" s="29">
         <v>982</v>
       </c>
-      <c r="F11" s="31">
-        <v>1101</v>
-      </c>
-      <c r="G11" s="32">
-        <v>1023</v>
+      <c r="F11" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>190</v>
       </c>
       <c r="H11" s="14"/>
       <c r="I11" s="15"/>
@@ -1396,14 +1691,14 @@
       <c r="B12" s="14"/>
       <c r="C12" s="15"/>
       <c r="D12" s="16"/>
-      <c r="E12" s="30">
+      <c r="E12" s="29">
         <v>1154</v>
       </c>
-      <c r="F12" s="37">
-        <v>512</v>
-      </c>
-      <c r="G12" s="32">
-        <v>538</v>
+      <c r="F12" s="34" t="s">
+        <v>210</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>191</v>
       </c>
       <c r="H12" s="14"/>
       <c r="I12" s="15"/>
@@ -1430,14 +1725,14 @@
       <c r="B13" s="14"/>
       <c r="C13" s="15"/>
       <c r="D13" s="16"/>
-      <c r="E13" s="30">
+      <c r="E13" s="29">
         <v>554</v>
       </c>
-      <c r="F13" s="35">
-        <v>399</v>
-      </c>
-      <c r="G13" s="36">
-        <v>401</v>
+      <c r="F13" s="34" t="s">
+        <v>211</v>
+      </c>
+      <c r="G13" s="35" t="s">
+        <v>192</v>
       </c>
       <c r="H13" s="14"/>
       <c r="I13" s="22"/>
@@ -1463,14 +1758,14 @@
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
       <c r="D14" s="16"/>
-      <c r="E14" s="30">
+      <c r="E14" s="29">
         <v>880</v>
       </c>
-      <c r="F14" s="31">
-        <v>712</v>
-      </c>
-      <c r="G14" s="32">
-        <v>897</v>
+      <c r="F14" s="30" t="s">
+        <v>212</v>
+      </c>
+      <c r="G14" s="31" t="s">
+        <v>193</v>
       </c>
       <c r="H14" s="14"/>
       <c r="I14" s="15"/>
@@ -1496,14 +1791,14 @@
       <c r="B15" s="14"/>
       <c r="C15" s="15"/>
       <c r="D15" s="16"/>
-      <c r="E15" s="30">
+      <c r="E15" s="29">
         <v>1549</v>
       </c>
-      <c r="F15" s="22">
-        <v>742</v>
-      </c>
-      <c r="G15" s="32">
-        <v>783</v>
+      <c r="F15" s="34" t="s">
+        <v>213</v>
+      </c>
+      <c r="G15" s="35" t="s">
+        <v>194</v>
       </c>
       <c r="H15" s="14"/>
       <c r="I15" s="15"/>
@@ -1529,14 +1824,14 @@
       <c r="B16" s="14"/>
       <c r="C16" s="15"/>
       <c r="D16" s="16"/>
-      <c r="E16" s="30">
+      <c r="E16" s="29">
         <v>1332</v>
       </c>
-      <c r="F16" s="31">
-        <v>946</v>
-      </c>
-      <c r="G16" s="32">
-        <v>886</v>
+      <c r="F16" s="36" t="s">
+        <v>214</v>
+      </c>
+      <c r="G16" s="33" t="s">
+        <v>195</v>
       </c>
       <c r="H16" s="14"/>
       <c r="I16" s="15"/>
@@ -1562,14 +1857,14 @@
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
       <c r="D17" s="16"/>
-      <c r="E17" s="30">
+      <c r="E17" s="29">
         <v>1227</v>
       </c>
-      <c r="F17" s="31">
-        <v>727</v>
-      </c>
-      <c r="G17" s="34">
-        <v>706</v>
+      <c r="F17" s="30" t="s">
+        <v>215</v>
+      </c>
+      <c r="G17" s="35" t="s">
+        <v>196</v>
       </c>
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
@@ -1595,14 +1890,14 @@
       <c r="B18" s="14"/>
       <c r="C18" s="15"/>
       <c r="D18" s="16"/>
-      <c r="E18" s="30">
+      <c r="E18" s="29">
         <v>4810</v>
       </c>
-      <c r="F18" s="31">
-        <v>3282</v>
-      </c>
-      <c r="G18" s="34">
-        <v>1918</v>
+      <c r="F18" s="36" t="s">
+        <v>216</v>
+      </c>
+      <c r="G18" s="33" t="s">
+        <v>197</v>
       </c>
       <c r="H18" s="14"/>
       <c r="I18" s="15"/>
@@ -1628,14 +1923,14 @@
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
       <c r="D19" s="16"/>
-      <c r="E19" s="30">
+      <c r="E19" s="29">
         <v>5232</v>
       </c>
-      <c r="F19" s="31">
-        <v>3849</v>
-      </c>
-      <c r="G19" s="34">
-        <v>2170</v>
+      <c r="F19" s="30" t="s">
+        <v>218</v>
+      </c>
+      <c r="G19" s="35" t="s">
+        <v>198</v>
       </c>
       <c r="H19" s="14"/>
       <c r="I19" s="15"/>
@@ -1663,14 +1958,14 @@
       <c r="B20" s="14"/>
       <c r="C20" s="15"/>
       <c r="D20" s="16"/>
-      <c r="E20" s="30">
+      <c r="E20" s="29">
         <v>5284</v>
       </c>
-      <c r="F20" s="31">
-        <v>3053</v>
-      </c>
-      <c r="G20" s="36">
-        <v>1749</v>
+      <c r="F20" s="34" t="s">
+        <v>217</v>
+      </c>
+      <c r="G20" s="35" t="s">
+        <v>199</v>
       </c>
       <c r="H20" s="14"/>
       <c r="I20" s="15"/>
@@ -1698,14 +1993,14 @@
       <c r="B21" s="14"/>
       <c r="C21" s="15"/>
       <c r="D21" s="16"/>
-      <c r="E21" s="30">
+      <c r="E21" s="29">
         <v>6039</v>
       </c>
-      <c r="F21" s="31">
-        <v>2584</v>
-      </c>
-      <c r="G21" s="36">
-        <v>1598</v>
+      <c r="F21" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="G21" s="35" t="s">
+        <v>200</v>
       </c>
       <c r="H21" s="14"/>
       <c r="I21" s="15"/>
@@ -1733,14 +2028,14 @@
       <c r="B22" s="14"/>
       <c r="C22" s="15"/>
       <c r="D22" s="16"/>
-      <c r="E22" s="30">
+      <c r="E22" s="29">
         <v>6214</v>
       </c>
-      <c r="F22" s="31">
-        <v>3849</v>
-      </c>
-      <c r="G22" s="34">
-        <v>1873</v>
+      <c r="F22" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="G22" s="35" t="s">
+        <v>201</v>
       </c>
       <c r="H22" s="14"/>
       <c r="I22" s="15"/>
@@ -1768,14 +2063,14 @@
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
       <c r="D23" s="16"/>
-      <c r="E23" s="30">
+      <c r="E23" s="29">
         <v>6206</v>
       </c>
-      <c r="F23" s="31">
-        <v>2976</v>
-      </c>
-      <c r="G23" s="34">
-        <v>1936</v>
+      <c r="F23" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="G23" s="35" t="s">
+        <v>202</v>
       </c>
       <c r="H23" s="14"/>
       <c r="I23" s="15"/>
@@ -1803,14 +2098,14 @@
       <c r="B24" s="17"/>
       <c r="C24" s="18"/>
       <c r="D24" s="19"/>
-      <c r="E24" s="33">
+      <c r="E24" s="32">
         <v>6198</v>
       </c>
-      <c r="F24" s="38">
-        <v>1905</v>
-      </c>
-      <c r="G24" s="39">
-        <v>1688</v>
+      <c r="F24" s="45" t="s">
+        <v>222</v>
+      </c>
+      <c r="G24" s="37" t="s">
+        <v>203</v>
       </c>
       <c r="H24" s="17"/>
       <c r="I24" s="18"/>
@@ -1841,11 +2136,11 @@
       <c r="E25" s="24">
         <v>633</v>
       </c>
-      <c r="F25" s="25">
-        <v>510</v>
-      </c>
-      <c r="G25" s="26">
-        <v>580</v>
+      <c r="F25" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="G25" s="26" t="s">
+        <v>126</v>
       </c>
       <c r="H25" s="24"/>
       <c r="I25" s="25"/>
@@ -1874,11 +2169,11 @@
       <c r="E26" s="11">
         <v>522</v>
       </c>
-      <c r="F26" s="7">
-        <v>475</v>
-      </c>
-      <c r="G26" s="8">
-        <v>529</v>
+      <c r="F26" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>156</v>
       </c>
       <c r="H26" s="11"/>
       <c r="I26" s="7"/>
@@ -1893,7 +2188,7 @@
       <c r="P26" s="11">
         <v>382</v>
       </c>
-      <c r="Q26" s="45">
+      <c r="Q26" s="38">
         <v>350</v>
       </c>
     </row>
@@ -1907,11 +2202,11 @@
       <c r="E27" s="11">
         <v>1273</v>
       </c>
-      <c r="F27" s="40">
-        <v>657</v>
-      </c>
-      <c r="G27" s="8">
-        <v>813</v>
+      <c r="F27" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>157</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="7"/>
@@ -1926,7 +2221,7 @@
       <c r="P27" s="11">
         <v>710</v>
       </c>
-      <c r="Q27" s="45">
+      <c r="Q27" s="38">
         <v>631</v>
       </c>
     </row>
@@ -1940,11 +2235,11 @@
       <c r="E28" s="11">
         <v>1388</v>
       </c>
-      <c r="F28" s="28">
-        <v>744</v>
-      </c>
-      <c r="G28" s="8">
-        <v>909</v>
+      <c r="F28" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>158</v>
       </c>
       <c r="H28" s="11"/>
       <c r="I28" s="7"/>
@@ -1959,7 +2254,7 @@
       <c r="P28" s="11">
         <v>653</v>
       </c>
-      <c r="Q28" s="45">
+      <c r="Q28" s="38">
         <v>607</v>
       </c>
     </row>
@@ -1973,11 +2268,11 @@
       <c r="E29" s="11">
         <v>1009</v>
       </c>
-      <c r="F29" s="28">
-        <v>730</v>
-      </c>
-      <c r="G29" s="8">
-        <v>644</v>
+      <c r="F29" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>159</v>
       </c>
       <c r="H29" s="11"/>
       <c r="I29" s="7"/>
@@ -1994,7 +2289,7 @@
       <c r="P29" s="11">
         <v>482</v>
       </c>
-      <c r="Q29" s="45">
+      <c r="Q29" s="38">
         <v>505</v>
       </c>
     </row>
@@ -2008,11 +2303,11 @@
       <c r="E30" s="11">
         <v>1181</v>
       </c>
-      <c r="F30" s="28">
-        <v>648</v>
-      </c>
-      <c r="G30" s="8">
-        <v>649</v>
+      <c r="F30" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>160</v>
       </c>
       <c r="H30" s="11"/>
       <c r="I30" s="7"/>
@@ -2029,7 +2324,7 @@
       <c r="P30" s="11">
         <v>489</v>
       </c>
-      <c r="Q30" s="45">
+      <c r="Q30" s="38">
         <v>497</v>
       </c>
     </row>
@@ -2043,11 +2338,11 @@
       <c r="E31" s="11">
         <v>2140</v>
       </c>
-      <c r="F31" s="28">
-        <v>1302</v>
-      </c>
-      <c r="G31" s="8">
-        <v>1315</v>
+      <c r="F31" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>161</v>
       </c>
       <c r="H31" s="11"/>
       <c r="I31" s="7"/>
@@ -2064,7 +2359,7 @@
       <c r="P31" s="11">
         <v>717</v>
       </c>
-      <c r="Q31" s="45">
+      <c r="Q31" s="38">
         <v>632</v>
       </c>
     </row>
@@ -2078,11 +2373,11 @@
       <c r="E32" s="11">
         <v>1697</v>
       </c>
-      <c r="F32" s="28">
-        <v>1475</v>
-      </c>
-      <c r="G32" s="8">
-        <v>1397</v>
+      <c r="F32" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>162</v>
       </c>
       <c r="H32" s="11"/>
       <c r="I32" s="7"/>
@@ -2099,7 +2394,7 @@
       <c r="P32" s="11">
         <v>847</v>
       </c>
-      <c r="Q32" s="45">
+      <c r="Q32" s="38">
         <v>706</v>
       </c>
     </row>
@@ -2113,11 +2408,11 @@
       <c r="E33" s="11">
         <v>977</v>
       </c>
-      <c r="F33" s="28">
-        <v>819</v>
-      </c>
-      <c r="G33" s="8">
-        <v>819</v>
+      <c r="F33" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>135</v>
       </c>
       <c r="H33" s="11"/>
       <c r="I33" s="7"/>
@@ -2134,7 +2429,7 @@
       <c r="P33" s="11">
         <v>535</v>
       </c>
-      <c r="Q33" s="45">
+      <c r="Q33" s="38">
         <v>533</v>
       </c>
     </row>
@@ -2148,11 +2443,11 @@
       <c r="E34" s="11">
         <v>1082</v>
       </c>
-      <c r="F34" s="28">
-        <v>959</v>
-      </c>
-      <c r="G34" s="8">
-        <v>740</v>
+      <c r="F34" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>163</v>
       </c>
       <c r="H34" s="11"/>
       <c r="I34" s="7"/>
@@ -2169,7 +2464,7 @@
       <c r="P34" s="11">
         <v>629</v>
       </c>
-      <c r="Q34" s="45">
+      <c r="Q34" s="38">
         <v>621</v>
       </c>
     </row>
@@ -2183,11 +2478,11 @@
       <c r="E35" s="11">
         <v>2653</v>
       </c>
-      <c r="F35" s="28">
-        <v>1258</v>
-      </c>
-      <c r="G35" s="8">
-        <v>1153</v>
+      <c r="F35" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>164</v>
       </c>
       <c r="H35" s="11"/>
       <c r="I35" s="7"/>
@@ -2204,7 +2499,7 @@
       <c r="P35" s="11">
         <v>708</v>
       </c>
-      <c r="Q35" s="45">
+      <c r="Q35" s="38">
         <v>767</v>
       </c>
     </row>
@@ -2218,11 +2513,11 @@
       <c r="E36" s="11">
         <v>2016</v>
       </c>
-      <c r="F36" s="28">
-        <v>1511</v>
-      </c>
-      <c r="G36" s="8">
-        <v>1357</v>
+      <c r="F36" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>165</v>
       </c>
       <c r="H36" s="11"/>
       <c r="I36" s="7"/>
@@ -2239,7 +2534,7 @@
       <c r="P36" s="11">
         <v>720</v>
       </c>
-      <c r="Q36" s="45">
+      <c r="Q36" s="38">
         <v>727</v>
       </c>
     </row>
@@ -2253,11 +2548,11 @@
       <c r="E37" s="11">
         <v>1401</v>
       </c>
-      <c r="F37" s="28">
-        <v>860</v>
-      </c>
-      <c r="G37" s="29">
-        <v>946</v>
+      <c r="F37" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="G37" s="40" t="s">
+        <v>166</v>
       </c>
       <c r="H37" s="11"/>
       <c r="I37" s="7"/>
@@ -2274,7 +2569,7 @@
       <c r="P37" s="11">
         <v>766</v>
       </c>
-      <c r="Q37" s="45">
+      <c r="Q37" s="38">
         <v>768</v>
       </c>
     </row>
@@ -2288,11 +2583,11 @@
       <c r="E38" s="11">
         <v>1796</v>
       </c>
-      <c r="F38" s="28">
-        <v>1003</v>
-      </c>
-      <c r="G38" s="8">
-        <v>1030</v>
+      <c r="F38" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>167</v>
       </c>
       <c r="H38" s="11"/>
       <c r="I38" s="7"/>
@@ -2309,7 +2604,7 @@
       <c r="P38" s="11">
         <v>871</v>
       </c>
-      <c r="Q38" s="45">
+      <c r="Q38" s="38">
         <v>888</v>
       </c>
     </row>
@@ -2323,11 +2618,11 @@
       <c r="E39" s="11">
         <v>2457</v>
       </c>
-      <c r="F39" s="28">
-        <v>1315</v>
-      </c>
-      <c r="G39" s="8">
-        <v>1281</v>
+      <c r="F39" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>168</v>
       </c>
       <c r="H39" s="11"/>
       <c r="I39" s="7"/>
@@ -2344,7 +2639,7 @@
       <c r="P39" s="11">
         <v>818</v>
       </c>
-      <c r="Q39" s="45">
+      <c r="Q39" s="38">
         <v>788</v>
       </c>
     </row>
@@ -2358,11 +2653,11 @@
       <c r="E40" s="11">
         <v>2547</v>
       </c>
-      <c r="F40" s="28">
-        <v>1535</v>
-      </c>
-      <c r="G40" s="8">
-        <v>1953</v>
+      <c r="F40" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>169</v>
       </c>
       <c r="H40" s="11"/>
       <c r="I40" s="7"/>
@@ -2379,7 +2674,7 @@
       <c r="P40" s="11">
         <v>831</v>
       </c>
-      <c r="Q40" s="45">
+      <c r="Q40" s="38">
         <v>808</v>
       </c>
     </row>
@@ -2393,11 +2688,11 @@
       <c r="E41" s="11">
         <v>1449</v>
       </c>
-      <c r="F41" s="28">
-        <v>1168</v>
-      </c>
-      <c r="G41" s="8">
-        <v>1222</v>
+      <c r="F41" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>170</v>
       </c>
       <c r="H41" s="11"/>
       <c r="I41" s="7"/>
@@ -2414,7 +2709,7 @@
       <c r="P41" s="11">
         <v>910</v>
       </c>
-      <c r="Q41" s="45">
+      <c r="Q41" s="38">
         <v>935</v>
       </c>
     </row>
@@ -2428,11 +2723,11 @@
       <c r="E42" s="11">
         <v>2089</v>
       </c>
-      <c r="F42" s="28">
-        <v>1312</v>
-      </c>
-      <c r="G42" s="8">
-        <v>1172</v>
+      <c r="F42" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>171</v>
       </c>
       <c r="H42" s="11"/>
       <c r="I42" s="7"/>
@@ -2449,7 +2744,7 @@
       <c r="P42" s="11">
         <v>951</v>
       </c>
-      <c r="Q42" s="45">
+      <c r="Q42" s="38">
         <v>939</v>
       </c>
     </row>
@@ -2463,11 +2758,11 @@
       <c r="E43" s="11">
         <v>1740</v>
       </c>
-      <c r="F43" s="28">
-        <v>1040</v>
-      </c>
-      <c r="G43" s="8">
-        <v>1011</v>
+      <c r="F43" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>172</v>
       </c>
       <c r="H43" s="11"/>
       <c r="I43" s="7"/>
@@ -2484,7 +2779,7 @@
       <c r="P43" s="11">
         <v>601</v>
       </c>
-      <c r="Q43" s="45">
+      <c r="Q43" s="38">
         <v>598</v>
       </c>
     </row>
@@ -2498,11 +2793,11 @@
       <c r="E44" s="11">
         <v>2345</v>
       </c>
-      <c r="F44" s="28">
-        <v>1315</v>
-      </c>
-      <c r="G44" s="8">
-        <v>1309</v>
+      <c r="F44" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>173</v>
       </c>
       <c r="H44" s="11"/>
       <c r="I44" s="7"/>
@@ -2519,7 +2814,7 @@
       <c r="P44" s="11">
         <v>815</v>
       </c>
-      <c r="Q44" s="45">
+      <c r="Q44" s="38">
         <v>854</v>
       </c>
     </row>
@@ -2533,11 +2828,11 @@
       <c r="E45" s="11">
         <v>1949</v>
       </c>
-      <c r="F45" s="28">
-        <v>1378</v>
-      </c>
-      <c r="G45" s="8">
-        <v>1365</v>
+      <c r="F45" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>174</v>
       </c>
       <c r="H45" s="11"/>
       <c r="I45" s="7"/>
@@ -2554,7 +2849,7 @@
       <c r="P45" s="11">
         <v>965</v>
       </c>
-      <c r="Q45" s="45">
+      <c r="Q45" s="38">
         <v>937</v>
       </c>
     </row>
@@ -2568,11 +2863,11 @@
       <c r="E46" s="11">
         <v>1985</v>
       </c>
-      <c r="F46" s="28">
-        <v>1603</v>
-      </c>
-      <c r="G46" s="8">
-        <v>1212</v>
+      <c r="F46" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>175</v>
       </c>
       <c r="H46" s="11"/>
       <c r="I46" s="7"/>
@@ -2589,7 +2884,7 @@
       <c r="P46" s="11">
         <v>902</v>
       </c>
-      <c r="Q46" s="45">
+      <c r="Q46" s="38">
         <v>826</v>
       </c>
     </row>
@@ -2603,11 +2898,11 @@
       <c r="E47" s="11">
         <v>1429</v>
       </c>
-      <c r="F47" s="28">
-        <v>1136</v>
-      </c>
-      <c r="G47" s="8">
-        <v>902</v>
+      <c r="F47" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>176</v>
       </c>
       <c r="H47" s="11"/>
       <c r="I47" s="7"/>
@@ -2624,7 +2919,7 @@
       <c r="P47" s="11">
         <v>632</v>
       </c>
-      <c r="Q47" s="45">
+      <c r="Q47" s="38">
         <v>548</v>
       </c>
     </row>
@@ -2638,11 +2933,11 @@
       <c r="E48" s="11">
         <v>1847</v>
       </c>
-      <c r="F48" s="28">
-        <v>1014</v>
-      </c>
-      <c r="G48" s="8">
-        <v>1037</v>
+      <c r="F48" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>177</v>
       </c>
       <c r="H48" s="11"/>
       <c r="I48" s="7"/>
@@ -2659,7 +2954,7 @@
       <c r="P48" s="11">
         <v>674</v>
       </c>
-      <c r="Q48" s="45">
+      <c r="Q48" s="38">
         <v>687</v>
       </c>
     </row>
@@ -2673,11 +2968,11 @@
       <c r="E49" s="11">
         <v>3083</v>
       </c>
-      <c r="F49" s="28">
-        <v>1201</v>
-      </c>
-      <c r="G49" s="8">
-        <v>1124</v>
+      <c r="F49" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>178</v>
       </c>
       <c r="H49" s="11"/>
       <c r="I49" s="7"/>
@@ -2694,7 +2989,7 @@
       <c r="P49" s="11">
         <v>897</v>
       </c>
-      <c r="Q49" s="45">
+      <c r="Q49" s="38">
         <v>885</v>
       </c>
     </row>
@@ -2708,11 +3003,11 @@
       <c r="E50" s="11">
         <v>2339</v>
       </c>
-      <c r="F50" s="28">
-        <v>1301</v>
-      </c>
-      <c r="G50" s="8">
-        <v>1450</v>
+      <c r="F50" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="G50" s="8" t="s">
+        <v>179</v>
       </c>
       <c r="H50" s="11"/>
       <c r="I50" s="7"/>
@@ -2729,7 +3024,7 @@
       <c r="P50" s="11">
         <v>903</v>
       </c>
-      <c r="Q50" s="45">
+      <c r="Q50" s="38">
         <v>915</v>
       </c>
     </row>
@@ -2743,11 +3038,11 @@
       <c r="E51" s="11">
         <v>2991</v>
       </c>
-      <c r="F51" s="28">
-        <v>1675</v>
-      </c>
-      <c r="G51" s="8">
-        <v>1638</v>
+      <c r="F51" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="G51" s="8" t="s">
+        <v>180</v>
       </c>
       <c r="H51" s="11"/>
       <c r="I51" s="7"/>
@@ -2764,7 +3059,7 @@
       <c r="P51" s="11">
         <v>981</v>
       </c>
-      <c r="Q51" s="45">
+      <c r="Q51" s="38">
         <v>982</v>
       </c>
     </row>
@@ -2778,11 +3073,11 @@
       <c r="E52" s="11">
         <v>2402</v>
       </c>
-      <c r="F52" s="28">
-        <v>1567</v>
-      </c>
-      <c r="G52" s="8">
-        <v>1210</v>
+      <c r="F52" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>181</v>
       </c>
       <c r="H52" s="11"/>
       <c r="I52" s="7"/>
@@ -2799,7 +3094,7 @@
       <c r="P52" s="11">
         <v>703</v>
       </c>
-      <c r="Q52" s="45">
+      <c r="Q52" s="38">
         <v>633</v>
       </c>
     </row>
@@ -2813,11 +3108,11 @@
       <c r="E53" s="11">
         <v>2843</v>
       </c>
-      <c r="F53" s="28">
-        <v>1993</v>
-      </c>
-      <c r="G53" s="8">
-        <v>1633</v>
+      <c r="F53" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="G53" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="H53" s="11"/>
       <c r="I53" s="7"/>
@@ -2834,7 +3129,7 @@
       <c r="P53" s="11">
         <v>760</v>
       </c>
-      <c r="Q53" s="45">
+      <c r="Q53" s="38">
         <v>800</v>
       </c>
     </row>
@@ -2848,11 +3143,11 @@
       <c r="E54" s="12">
         <v>2637</v>
       </c>
-      <c r="F54" s="9">
-        <v>1084</v>
-      </c>
-      <c r="G54" s="10">
-        <v>1073</v>
+      <c r="F54" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="G54" s="10" t="s">
+        <v>183</v>
       </c>
       <c r="H54" s="12"/>
       <c r="I54" s="9"/>
@@ -2879,9 +3174,9 @@
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:G3"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="K3:M3"/>
+    <mergeCell ref="E3:G3"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Reduced size of neighbourhood solutions returned from TS
</commit_message>
<xml_diff>
--- a/data/Benchmarks/MKS.xlsx
+++ b/data/Benchmarks/MKS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\MSTS_FJSP\data\Benchmarks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2459ACD7-E8A5-40F2-8700-E89860EEF0CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BC2E9A-9B1E-489F-BAE2-78238E35F964}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{87D6751E-06B1-440E-A7B4-B38AD42E9B96}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{87D6751E-06B1-440E-A7B4-B38AD42E9B96}"/>
   </bookViews>
   <sheets>
     <sheet name="Birgin Test Cases" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="180">
   <si>
     <t>SMT</t>
   </si>
@@ -819,7 +819,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -956,13 +956,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -977,9 +980,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1444,6 +1445,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-0680-4033-8D19-0774B908C676}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="19"/>
@@ -1458,6 +1464,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-0680-4033-8D19-0774B908C676}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -5130,8 +5141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42C717E4-2E19-4E10-82CD-C66DD0E858F2}">
   <dimension ref="A1:Y61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AP21" sqref="AP21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5145,77 +5156,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="74" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="70"/>
-      <c r="N3" s="70"/>
-      <c r="O3" s="70"/>
-      <c r="P3" s="71"/>
-      <c r="Q3" s="72" t="s">
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="73"/>
+      <c r="N3" s="73"/>
+      <c r="O3" s="73"/>
+      <c r="P3" s="72"/>
+      <c r="Q3" s="71" t="s">
         <v>177</v>
       </c>
-      <c r="R3" s="71"/>
-      <c r="S3" s="70" t="s">
+      <c r="R3" s="72"/>
+      <c r="S3" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="T3" s="71"/>
-      <c r="U3" s="72" t="s">
+      <c r="T3" s="72"/>
+      <c r="U3" s="71" t="s">
         <v>172</v>
       </c>
-      <c r="V3" s="71"/>
+      <c r="V3" s="72"/>
       <c r="W3" s="6"/>
       <c r="X3" s="7"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="72" t="s">
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="70"/>
-      <c r="I4" s="70"/>
-      <c r="J4" s="70"/>
-      <c r="K4" s="71"/>
-      <c r="L4" s="72" t="s">
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="70"/>
-      <c r="N4" s="70"/>
-      <c r="O4" s="70"/>
-      <c r="P4" s="71"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="73"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="72"/>
       <c r="Q4" s="3" t="s">
         <v>5</v>
       </c>
@@ -5237,7 +5248,7 @@
       <c r="W4" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="X4" s="77"/>
+      <c r="X4" s="70"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="40" t="s">
@@ -6765,61 +6776,61 @@
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
-      <c r="B27" s="72" t="s">
+      <c r="B27" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="70"/>
-      <c r="D27" s="70"/>
-      <c r="E27" s="70"/>
-      <c r="F27" s="70"/>
-      <c r="G27" s="70"/>
-      <c r="H27" s="70"/>
-      <c r="I27" s="70"/>
-      <c r="J27" s="70"/>
-      <c r="K27" s="70"/>
-      <c r="L27" s="70"/>
-      <c r="M27" s="70"/>
-      <c r="N27" s="70"/>
-      <c r="O27" s="70"/>
-      <c r="P27" s="71"/>
-      <c r="Q27" s="72" t="s">
+      <c r="C27" s="73"/>
+      <c r="D27" s="73"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="73"/>
+      <c r="H27" s="73"/>
+      <c r="I27" s="73"/>
+      <c r="J27" s="73"/>
+      <c r="K27" s="73"/>
+      <c r="L27" s="73"/>
+      <c r="M27" s="73"/>
+      <c r="N27" s="73"/>
+      <c r="O27" s="73"/>
+      <c r="P27" s="72"/>
+      <c r="Q27" s="71" t="s">
         <v>177</v>
       </c>
-      <c r="R27" s="71"/>
-      <c r="S27" s="70" t="s">
+      <c r="R27" s="72"/>
+      <c r="S27" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="T27" s="71"/>
-      <c r="U27" s="72" t="s">
+      <c r="T27" s="72"/>
+      <c r="U27" s="71" t="s">
         <v>172</v>
       </c>
-      <c r="V27" s="71"/>
+      <c r="V27" s="72"/>
       <c r="W27" s="11"/>
       <c r="X27" s="7"/>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
-      <c r="B28" s="72" t="s">
+      <c r="B28" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="C28" s="70"/>
-      <c r="D28" s="70"/>
-      <c r="E28" s="70"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="72" t="s">
+      <c r="C28" s="73"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="73"/>
+      <c r="F28" s="72"/>
+      <c r="G28" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="H28" s="70"/>
-      <c r="I28" s="70"/>
-      <c r="J28" s="70"/>
-      <c r="K28" s="71"/>
-      <c r="L28" s="72" t="s">
+      <c r="H28" s="73"/>
+      <c r="I28" s="73"/>
+      <c r="J28" s="73"/>
+      <c r="K28" s="72"/>
+      <c r="L28" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="M28" s="70"/>
-      <c r="N28" s="70"/>
-      <c r="O28" s="70"/>
-      <c r="P28" s="71"/>
+      <c r="M28" s="73"/>
+      <c r="N28" s="73"/>
+      <c r="O28" s="73"/>
+      <c r="P28" s="72"/>
       <c r="Q28" s="3" t="s">
         <v>5</v>
       </c>
@@ -6839,7 +6850,7 @@
         <v>174</v>
       </c>
       <c r="W28" s="63"/>
-      <c r="X28" s="77"/>
+      <c r="X28" s="70"/>
       <c r="Y28" s="7"/>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.3">
@@ -8989,21 +9000,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="S27:T27"/>
+    <mergeCell ref="U27:V27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="G28:K28"/>
+    <mergeCell ref="L28:P28"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="L4:P4"/>
+    <mergeCell ref="B27:P27"/>
+    <mergeCell ref="Q27:R27"/>
     <mergeCell ref="U3:V3"/>
     <mergeCell ref="S3:T3"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="Q3:R3"/>
     <mergeCell ref="B3:P3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="G4:K4"/>
-    <mergeCell ref="L4:P4"/>
-    <mergeCell ref="B27:P27"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="S27:T27"/>
-    <mergeCell ref="U27:V27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="G28:K28"/>
-    <mergeCell ref="L28:P28"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9023,37 +9034,37 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="74" t="s">
         <v>153</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="72" t="s">
+      <c r="C3" s="73"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="72" t="s">
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="71" t="s">
         <v>121</v>
       </c>
-      <c r="I3" s="70"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="72" t="s">
+      <c r="I3" s="73"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="71" t="s">
         <v>154</v>
       </c>
-      <c r="L3" s="71"/>
+      <c r="L3" s="72"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
@@ -9406,10 +9417,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{849930BA-C1CC-4AFE-B573-763F33389D3C}">
-  <dimension ref="A1:P28"/>
+  <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9417,871 +9428,1395 @@
     <col min="11" max="11" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="73" t="s">
+    <row r="1" spans="1:22" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="74" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
-      <c r="B3" s="72" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="72" t="s">
+      <c r="B3" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="72" t="s">
-        <v>121</v>
-      </c>
-      <c r="I3" s="70"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="72" t="s">
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="73"/>
+      <c r="N3" s="73"/>
+      <c r="O3" s="73"/>
+      <c r="P3" s="72"/>
+      <c r="Q3" s="71" t="s">
         <v>145</v>
       </c>
-      <c r="L3" s="71"/>
-      <c r="M3" s="74" t="s">
+      <c r="R3" s="72"/>
+      <c r="S3" s="75" t="s">
         <v>151</v>
       </c>
-      <c r="N3" s="75"/>
-      <c r="O3" s="75"/>
-      <c r="P3" s="76"/>
+      <c r="T3" s="76"/>
+      <c r="U3" s="76"/>
+      <c r="V3" s="77"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="M4" s="73"/>
+      <c r="N4" s="73"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="72"/>
+      <c r="Q4" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="23">
+        <v>91</v>
+      </c>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="43">
+        <f>(B5-C5)/B5</f>
+        <v>1</v>
+      </c>
+      <c r="G5" s="24">
+        <v>91</v>
+      </c>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42">
+        <f>(G5-H5)/G5</f>
+        <v>1</v>
+      </c>
+      <c r="J5" s="69">
+        <v>66</v>
+      </c>
+      <c r="K5" s="43">
+        <f>(G5-J5)/G5</f>
+        <v>0.27472527472527475</v>
+      </c>
+      <c r="L5" s="25">
+        <v>91</v>
+      </c>
+      <c r="M5" s="42"/>
+      <c r="N5" s="42">
+        <f>(L5-M5)/L5</f>
+        <v>1</v>
+      </c>
+      <c r="O5" s="69">
+        <v>66</v>
+      </c>
+      <c r="P5" s="43">
+        <f>(L5-O5)/L5</f>
+        <v>0.27472527472527475</v>
+      </c>
+      <c r="Q5" s="19">
+        <v>66</v>
+      </c>
+      <c r="R5" s="20">
+        <v>66</v>
+      </c>
+      <c r="S5" s="11">
+        <v>66</v>
+      </c>
+      <c r="T5" s="7">
+        <v>66</v>
+      </c>
+      <c r="U5" s="35">
+        <v>66</v>
+      </c>
+      <c r="V5" s="8">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="23">
+        <v>128</v>
+      </c>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="8">
+        <f t="shared" ref="F6:F18" si="0">(B6-C6)/B6</f>
+        <v>1</v>
+      </c>
+      <c r="G6" s="24">
+        <v>128</v>
+      </c>
+      <c r="H6" s="49"/>
+      <c r="I6" s="42">
+        <f>(G6-H6)/G6</f>
+        <v>1</v>
+      </c>
+      <c r="J6" s="49">
+        <v>107</v>
+      </c>
+      <c r="K6" s="43">
+        <f>(G6-J6)/G6</f>
+        <v>0.1640625</v>
+      </c>
+      <c r="L6" s="25">
+        <v>128</v>
+      </c>
+      <c r="M6" s="49"/>
+      <c r="N6" s="7">
+        <f t="shared" ref="N6:N24" si="1">(L6-M6)/L6</f>
+        <v>1</v>
+      </c>
+      <c r="O6" s="49">
+        <v>107</v>
+      </c>
+      <c r="P6" s="8">
+        <f t="shared" ref="P6:P24" si="2">(L6-O6)/L6</f>
+        <v>0.1640625</v>
+      </c>
+      <c r="Q6" s="13">
+        <v>107</v>
+      </c>
+      <c r="R6" s="15">
+        <v>107</v>
+      </c>
+      <c r="S6" s="11">
+        <v>107</v>
+      </c>
+      <c r="T6" s="35">
+        <v>107</v>
+      </c>
+      <c r="U6" s="35">
+        <v>107</v>
+      </c>
+      <c r="V6" s="32">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="23">
+        <v>298</v>
+      </c>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G7" s="24">
+        <v>298</v>
+      </c>
+      <c r="H7" s="49"/>
+      <c r="I7" s="42">
+        <f>(G7-H7)/G7</f>
+        <v>1</v>
+      </c>
+      <c r="J7" s="78">
+        <v>236</v>
+      </c>
+      <c r="K7" s="43">
+        <f>(G7-J7)/G7</f>
+        <v>0.20805369127516779</v>
+      </c>
+      <c r="L7" s="25">
+        <v>298</v>
+      </c>
+      <c r="M7" s="49"/>
+      <c r="N7" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O7" s="49">
+        <v>221</v>
+      </c>
+      <c r="P7" s="8">
+        <f t="shared" si="2"/>
+        <v>0.25838926174496646</v>
+      </c>
+      <c r="Q7" s="13">
+        <v>221</v>
+      </c>
+      <c r="R7" s="15">
+        <v>221</v>
+      </c>
+      <c r="S7" s="11">
+        <v>221</v>
+      </c>
+      <c r="T7" s="7">
+        <v>221</v>
+      </c>
+      <c r="U7" s="7">
+        <v>221</v>
+      </c>
+      <c r="V7" s="8">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="23">
+        <v>396</v>
+      </c>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G8" s="24">
+        <v>396</v>
+      </c>
+      <c r="H8" s="49"/>
+      <c r="I8" s="42">
+        <f>(G8-H8)/G8</f>
+        <v>1</v>
+      </c>
+      <c r="J8" s="49">
+        <v>355</v>
+      </c>
+      <c r="K8" s="43">
+        <f>(G8-J8)/G8</f>
+        <v>0.10353535353535354</v>
+      </c>
+      <c r="L8" s="25">
+        <v>396</v>
+      </c>
+      <c r="M8" s="49"/>
+      <c r="N8" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O8" s="49">
+        <v>355</v>
+      </c>
+      <c r="P8" s="8">
+        <f t="shared" si="2"/>
+        <v>0.10353535353535354</v>
+      </c>
+      <c r="Q8" s="13">
+        <v>355</v>
+      </c>
+      <c r="R8" s="15">
+        <v>355</v>
+      </c>
+      <c r="S8" s="11">
+        <v>355</v>
+      </c>
+      <c r="T8" s="7">
+        <v>355</v>
+      </c>
+      <c r="U8" s="7">
+        <v>355</v>
+      </c>
+      <c r="V8" s="8">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="23">
+        <v>119</v>
+      </c>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G9" s="21">
+        <v>119</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="42">
+        <f>(G9-H9)/G9</f>
+        <v>1</v>
+      </c>
+      <c r="J9" s="49">
+        <v>119</v>
+      </c>
+      <c r="K9" s="43">
+        <f>(G9-J9)/G9</f>
         <v>0</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="L9" s="22">
+        <v>119</v>
+      </c>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="O9" s="65">
+        <v>119</v>
+      </c>
+      <c r="P9" s="8">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="Q9" s="13">
+        <v>119</v>
+      </c>
+      <c r="R9" s="15">
+        <v>119</v>
+      </c>
+      <c r="S9" s="11">
+        <v>119</v>
+      </c>
+      <c r="T9" s="7">
+        <v>119</v>
+      </c>
+      <c r="U9" s="7">
+        <v>119</v>
+      </c>
+      <c r="V9" s="8">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" s="23">
+        <v>360</v>
+      </c>
+      <c r="C10" s="64"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="8">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>149</v>
+      <c r="G10" s="24">
+        <v>360</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="42">
+        <f>(G10-H10)/G10</f>
+        <v>1</v>
+      </c>
+      <c r="J10" s="49">
+        <v>320</v>
+      </c>
+      <c r="K10" s="43">
+        <f>(G10-J10)/G10</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="L10" s="25">
+        <v>360</v>
+      </c>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O10" s="65">
+        <v>320</v>
+      </c>
+      <c r="P10" s="8">
+        <f t="shared" si="2"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="Q10" s="13">
+        <v>320</v>
+      </c>
+      <c r="R10" s="15">
+        <v>320</v>
+      </c>
+      <c r="S10" s="11">
+        <v>320</v>
+      </c>
+      <c r="T10" s="7">
+        <v>320</v>
+      </c>
+      <c r="U10" s="7">
+        <v>320</v>
+      </c>
+      <c r="V10" s="8">
+        <v>320</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="23">
-        <v>91</v>
-      </c>
-      <c r="F5" s="24">
-        <v>91</v>
-      </c>
-      <c r="G5" s="25">
-        <v>91</v>
-      </c>
-      <c r="H5" s="23"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="19">
-        <v>66</v>
-      </c>
-      <c r="L5" s="20">
-        <v>66</v>
-      </c>
-      <c r="M5" s="11">
-        <v>66</v>
-      </c>
-      <c r="N5" s="7">
-        <v>66</v>
-      </c>
-      <c r="O5" s="35">
-        <v>66</v>
-      </c>
-      <c r="P5" s="8">
-        <v>66</v>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B11" s="23">
+        <v>397</v>
+      </c>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G11" s="21">
+        <v>397</v>
+      </c>
+      <c r="H11" s="7"/>
+      <c r="I11" s="42">
+        <f>(G11-H11)/G11</f>
+        <v>1</v>
+      </c>
+      <c r="J11" s="49">
+        <v>397</v>
+      </c>
+      <c r="K11" s="43">
+        <f>(G11-J11)/G11</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="22">
+        <v>397</v>
+      </c>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O11" s="65">
+        <v>397</v>
+      </c>
+      <c r="P11" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="13">
+        <v>397</v>
+      </c>
+      <c r="R11" s="15">
+        <v>397</v>
+      </c>
+      <c r="S11" s="11">
+        <v>397</v>
+      </c>
+      <c r="T11" s="7">
+        <v>397</v>
+      </c>
+      <c r="U11" s="7">
+        <v>397</v>
+      </c>
+      <c r="V11" s="8">
+        <v>397</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="23">
-        <v>128</v>
-      </c>
-      <c r="F6" s="24">
-        <v>128</v>
-      </c>
-      <c r="G6" s="25">
-        <v>128</v>
-      </c>
-      <c r="H6" s="23"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="13">
-        <v>107</v>
-      </c>
-      <c r="L6" s="15">
-        <v>107</v>
-      </c>
-      <c r="M6" s="11">
-        <v>107</v>
-      </c>
-      <c r="N6" s="35">
-        <v>107</v>
-      </c>
-      <c r="O6" s="35">
-        <v>107</v>
-      </c>
-      <c r="P6" s="32">
-        <v>107</v>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" s="23">
+        <v>325</v>
+      </c>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G12" s="24">
+        <v>325</v>
+      </c>
+      <c r="H12" s="49"/>
+      <c r="I12" s="42">
+        <f>(G12-H12)/G12</f>
+        <v>1</v>
+      </c>
+      <c r="J12" s="49">
+        <v>253</v>
+      </c>
+      <c r="K12" s="43">
+        <f>(G12-J12)/G12</f>
+        <v>0.22153846153846155</v>
+      </c>
+      <c r="L12" s="25">
+        <v>325</v>
+      </c>
+      <c r="M12" s="49"/>
+      <c r="N12" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O12" s="49">
+        <v>253</v>
+      </c>
+      <c r="P12" s="8">
+        <f t="shared" si="2"/>
+        <v>0.22153846153846155</v>
+      </c>
+      <c r="Q12" s="13">
+        <v>253</v>
+      </c>
+      <c r="R12" s="15">
+        <v>253</v>
+      </c>
+      <c r="S12" s="11">
+        <v>253</v>
+      </c>
+      <c r="T12" s="7">
+        <v>253</v>
+      </c>
+      <c r="U12" s="7">
+        <v>253</v>
+      </c>
+      <c r="V12" s="8">
+        <v>256</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="23">
-        <v>298</v>
-      </c>
-      <c r="F7" s="24">
-        <v>298</v>
-      </c>
-      <c r="G7" s="25">
-        <v>298</v>
-      </c>
-      <c r="H7" s="23"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="13">
-        <v>221</v>
-      </c>
-      <c r="L7" s="15">
-        <v>221</v>
-      </c>
-      <c r="M7" s="11">
-        <v>221</v>
-      </c>
-      <c r="N7" s="7">
-        <v>221</v>
-      </c>
-      <c r="O7" s="7">
-        <v>221</v>
-      </c>
-      <c r="P7" s="8">
-        <v>221</v>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" s="23">
+        <v>257</v>
+      </c>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G13" s="24">
+        <v>290</v>
+      </c>
+      <c r="H13" s="49"/>
+      <c r="I13" s="42">
+        <f>(G13-H13)/G13</f>
+        <v>1</v>
+      </c>
+      <c r="J13" s="78">
+        <v>220</v>
+      </c>
+      <c r="K13" s="43">
+        <f>(G13-J13)/G13</f>
+        <v>0.2413793103448276</v>
+      </c>
+      <c r="L13" s="25">
+        <v>257</v>
+      </c>
+      <c r="M13" s="49"/>
+      <c r="N13" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O13" s="49">
+        <v>210</v>
+      </c>
+      <c r="P13" s="8">
+        <f t="shared" si="2"/>
+        <v>0.1828793774319066</v>
+      </c>
+      <c r="Q13" s="13">
+        <v>210</v>
+      </c>
+      <c r="R13" s="15">
+        <v>210</v>
+      </c>
+      <c r="S13" s="11">
+        <v>210</v>
+      </c>
+      <c r="T13" s="7">
+        <v>210</v>
+      </c>
+      <c r="U13" s="7">
+        <v>210</v>
+      </c>
+      <c r="V13" s="8">
+        <v>210</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="23">
-        <v>396</v>
-      </c>
-      <c r="F8" s="24">
-        <v>396</v>
-      </c>
-      <c r="G8" s="25">
-        <v>396</v>
-      </c>
-      <c r="H8" s="23"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="13">
-        <v>355</v>
-      </c>
-      <c r="L8" s="15">
-        <v>355</v>
-      </c>
-      <c r="M8" s="11">
-        <v>355</v>
-      </c>
-      <c r="N8" s="7">
-        <v>355</v>
-      </c>
-      <c r="O8" s="7">
-        <v>355</v>
-      </c>
-      <c r="P8" s="8">
-        <v>355</v>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" s="26">
+        <v>516</v>
+      </c>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G14" s="36">
+        <v>516</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="42">
+        <f>(G14-H14)/G14</f>
+        <v>1</v>
+      </c>
+      <c r="J14" s="49">
+        <v>516</v>
+      </c>
+      <c r="K14" s="43">
+        <f>(G14-J14)/G14</f>
+        <v>0</v>
+      </c>
+      <c r="L14" s="37">
+        <v>516</v>
+      </c>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O14" s="65">
+        <v>516</v>
+      </c>
+      <c r="P14" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="16">
+        <v>516</v>
+      </c>
+      <c r="R14" s="18">
+        <v>516</v>
+      </c>
+      <c r="S14" s="12">
+        <v>516</v>
+      </c>
+      <c r="T14" s="9">
+        <v>516</v>
+      </c>
+      <c r="U14" s="9">
+        <v>516</v>
+      </c>
+      <c r="V14" s="10">
+        <v>519</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="23">
-        <v>119</v>
-      </c>
-      <c r="F9" s="21">
-        <v>119</v>
-      </c>
-      <c r="G9" s="22">
-        <v>119</v>
-      </c>
-      <c r="H9" s="23"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="13">
-        <v>119</v>
-      </c>
-      <c r="L9" s="15">
-        <v>119</v>
-      </c>
-      <c r="M9" s="11">
-        <v>119</v>
-      </c>
-      <c r="N9" s="7">
-        <v>119</v>
-      </c>
-      <c r="O9" s="7">
-        <v>119</v>
-      </c>
-      <c r="P9" s="8">
-        <v>119</v>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A15" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="B15" s="23">
+        <v>719</v>
+      </c>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G15" s="24">
+        <v>664</v>
+      </c>
+      <c r="H15" s="49"/>
+      <c r="I15" s="42">
+        <f>(G15-H15)/G15</f>
+        <v>1</v>
+      </c>
+      <c r="J15" s="78">
+        <v>479</v>
+      </c>
+      <c r="K15" s="43">
+        <f>(G15-J15)/G15</f>
+        <v>0.27861445783132532</v>
+      </c>
+      <c r="L15" s="25">
+        <v>664</v>
+      </c>
+      <c r="M15" s="49"/>
+      <c r="N15" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O15" s="78">
+        <v>495</v>
+      </c>
+      <c r="P15" s="8">
+        <f t="shared" si="2"/>
+        <v>0.25451807228915663</v>
+      </c>
+      <c r="Q15" s="13">
+        <v>468</v>
+      </c>
+      <c r="R15" s="15">
+        <v>468</v>
+      </c>
+      <c r="S15" s="11">
+        <v>479</v>
+      </c>
+      <c r="T15" s="7">
+        <v>491</v>
+      </c>
+      <c r="U15" s="7">
+        <v>469</v>
+      </c>
+      <c r="V15" s="8">
+        <v>469</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="23">
-        <v>360</v>
-      </c>
-      <c r="F10" s="24">
-        <v>360</v>
-      </c>
-      <c r="G10" s="25">
-        <v>360</v>
-      </c>
-      <c r="H10" s="23"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="13">
-        <v>320</v>
-      </c>
-      <c r="L10" s="15">
-        <v>320</v>
-      </c>
-      <c r="M10" s="11">
-        <v>320</v>
-      </c>
-      <c r="N10" s="7">
-        <v>320</v>
-      </c>
-      <c r="O10" s="7">
-        <v>320</v>
-      </c>
-      <c r="P10" s="8">
-        <v>320</v>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" s="23">
+        <v>628</v>
+      </c>
+      <c r="C16" s="66"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G16" s="24">
+        <v>571</v>
+      </c>
+      <c r="H16" s="51"/>
+      <c r="I16" s="42">
+        <f>(G16-H16)/G16</f>
+        <v>1</v>
+      </c>
+      <c r="J16" s="78">
+        <v>459</v>
+      </c>
+      <c r="K16" s="43">
+        <f>(G16-J16)/G16</f>
+        <v>0.19614711033274956</v>
+      </c>
+      <c r="L16" s="25">
+        <v>586</v>
+      </c>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O16" s="68">
+        <v>466</v>
+      </c>
+      <c r="P16" s="8">
+        <f t="shared" si="2"/>
+        <v>0.20477815699658702</v>
+      </c>
+      <c r="Q16" s="13">
+        <v>446</v>
+      </c>
+      <c r="R16" s="15">
+        <v>446</v>
+      </c>
+      <c r="S16" s="11">
+        <v>495</v>
+      </c>
+      <c r="T16" s="35">
+        <v>482</v>
+      </c>
+      <c r="U16" s="35">
+        <v>482</v>
+      </c>
+      <c r="V16" s="8">
+        <v>468</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="23">
-        <v>397</v>
-      </c>
-      <c r="F11" s="21">
-        <v>397</v>
-      </c>
-      <c r="G11" s="22">
-        <v>397</v>
-      </c>
-      <c r="H11" s="23"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="13">
-        <v>397</v>
-      </c>
-      <c r="L11" s="15">
-        <v>397</v>
-      </c>
-      <c r="M11" s="11">
-        <v>397</v>
-      </c>
-      <c r="N11" s="7">
-        <v>397</v>
-      </c>
-      <c r="O11" s="7">
-        <v>397</v>
-      </c>
-      <c r="P11" s="8">
-        <v>397</v>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B17" s="23">
+        <v>761</v>
+      </c>
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G17" s="24">
+        <v>731</v>
+      </c>
+      <c r="H17" s="51"/>
+      <c r="I17" s="42">
+        <f>(G17-H17)/G17</f>
+        <v>1</v>
+      </c>
+      <c r="J17" s="78">
+        <v>473</v>
+      </c>
+      <c r="K17" s="43">
+        <f>(G17-J17)/G17</f>
+        <v>0.35294117647058826</v>
+      </c>
+      <c r="L17" s="25">
+        <v>723</v>
+      </c>
+      <c r="M17" s="49"/>
+      <c r="N17" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O17" s="78">
+        <v>479</v>
+      </c>
+      <c r="P17" s="8">
+        <f t="shared" si="2"/>
+        <v>0.33748271092669435</v>
+      </c>
+      <c r="Q17" s="13">
+        <v>466</v>
+      </c>
+      <c r="R17" s="15">
+        <v>466</v>
+      </c>
+      <c r="S17" s="11">
+        <v>553</v>
+      </c>
+      <c r="T17" s="35">
+        <v>538</v>
+      </c>
+      <c r="U17" s="35">
+        <v>533</v>
+      </c>
+      <c r="V17" s="8">
+        <v>538</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="23">
-        <v>325</v>
-      </c>
-      <c r="F12" s="24">
-        <v>325</v>
-      </c>
-      <c r="G12" s="25">
-        <v>325</v>
-      </c>
-      <c r="H12" s="23"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="13">
-        <v>253</v>
-      </c>
-      <c r="L12" s="15">
-        <v>253</v>
-      </c>
-      <c r="M12" s="11">
-        <v>253</v>
-      </c>
-      <c r="N12" s="7">
-        <v>253</v>
-      </c>
-      <c r="O12" s="7">
-        <v>253</v>
-      </c>
-      <c r="P12" s="8">
-        <v>256</v>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B18" s="23">
+        <v>891</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G18" s="24">
+        <v>851</v>
+      </c>
+      <c r="H18" s="51"/>
+      <c r="I18" s="42">
+        <f>(G18-H18)/G18</f>
+        <v>1</v>
+      </c>
+      <c r="J18" s="78">
+        <v>572</v>
+      </c>
+      <c r="K18" s="43">
+        <f>(G18-J18)/G18</f>
+        <v>0.32784958871915393</v>
+      </c>
+      <c r="L18" s="25">
+        <v>816</v>
+      </c>
+      <c r="M18" s="51"/>
+      <c r="N18" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O18" s="78">
+        <v>567</v>
+      </c>
+      <c r="P18" s="8">
+        <f t="shared" si="2"/>
+        <v>0.30514705882352944</v>
+      </c>
+      <c r="Q18" s="13">
+        <v>554</v>
+      </c>
+      <c r="R18" s="15">
+        <v>554</v>
+      </c>
+      <c r="S18" s="11">
+        <v>656</v>
+      </c>
+      <c r="T18" s="35">
+        <v>650</v>
+      </c>
+      <c r="U18" s="35">
+        <v>634</v>
+      </c>
+      <c r="V18" s="8">
+        <v>618</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="23">
-        <v>257</v>
-      </c>
-      <c r="F13" s="24">
-        <v>290</v>
-      </c>
-      <c r="G13" s="25">
-        <v>257</v>
-      </c>
-      <c r="H13" s="23"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="13">
-        <v>210</v>
-      </c>
-      <c r="L13" s="15">
-        <v>210</v>
-      </c>
-      <c r="M13" s="11">
-        <v>210</v>
-      </c>
-      <c r="N13" s="7">
-        <v>210</v>
-      </c>
-      <c r="O13" s="7">
-        <v>210</v>
-      </c>
-      <c r="P13" s="8">
-        <v>210</v>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B19" s="23">
+        <v>815</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="G19" s="24">
+        <v>762</v>
+      </c>
+      <c r="H19" s="7"/>
+      <c r="I19" s="42">
+        <f>(G19-H19)/G19</f>
+        <v>1</v>
+      </c>
+      <c r="J19" s="78">
+        <v>584</v>
+      </c>
+      <c r="K19" s="43">
+        <f>(G19-J19)/G19</f>
+        <v>0.23359580052493439</v>
+      </c>
+      <c r="L19" s="25">
+        <v>784</v>
+      </c>
+      <c r="M19" s="49"/>
+      <c r="N19" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O19" s="78">
+        <v>561</v>
+      </c>
+      <c r="P19" s="8">
+        <f t="shared" si="2"/>
+        <v>0.28443877551020408</v>
+      </c>
+      <c r="Q19" s="13">
+        <v>514</v>
+      </c>
+      <c r="R19" s="15">
+        <v>514</v>
+      </c>
+      <c r="S19" s="11">
+        <v>650</v>
+      </c>
+      <c r="T19" s="35">
+        <v>662</v>
+      </c>
+      <c r="U19" s="35">
+        <v>625</v>
+      </c>
+      <c r="V19" s="8">
+        <v>625</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="26">
-        <v>516</v>
-      </c>
-      <c r="F14" s="36">
-        <v>516</v>
-      </c>
-      <c r="G14" s="37">
-        <v>516</v>
-      </c>
-      <c r="H14" s="26"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="16">
-        <v>516</v>
-      </c>
-      <c r="L14" s="18">
-        <v>516</v>
-      </c>
-      <c r="M14" s="12">
-        <v>516</v>
-      </c>
-      <c r="N14" s="9">
-        <v>516</v>
-      </c>
-      <c r="O14" s="9">
-        <v>516</v>
-      </c>
-      <c r="P14" s="10">
-        <v>519</v>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B20" s="23">
+        <v>960</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="G20" s="24">
+        <v>826</v>
+      </c>
+      <c r="H20" s="49"/>
+      <c r="I20" s="42">
+        <f>(G20-H20)/G20</f>
+        <v>1</v>
+      </c>
+      <c r="J20" s="78">
+        <v>700</v>
+      </c>
+      <c r="K20" s="43">
+        <f>(G20-J20)/G20</f>
+        <v>0.15254237288135594</v>
+      </c>
+      <c r="L20" s="25">
+        <v>879</v>
+      </c>
+      <c r="M20" s="49"/>
+      <c r="N20" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O20" s="78">
+        <v>650</v>
+      </c>
+      <c r="P20" s="8">
+        <f t="shared" si="2"/>
+        <v>0.26052332195676908</v>
+      </c>
+      <c r="Q20" s="13">
+        <v>608</v>
+      </c>
+      <c r="R20" s="15">
+        <v>608</v>
+      </c>
+      <c r="S20" s="11">
+        <v>762</v>
+      </c>
+      <c r="T20" s="35">
+        <v>785</v>
+      </c>
+      <c r="U20" s="35">
+        <v>717</v>
+      </c>
+      <c r="V20" s="8">
+        <v>730</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="23">
-        <v>719</v>
-      </c>
-      <c r="F15" s="24">
-        <v>664</v>
-      </c>
-      <c r="G15" s="25">
-        <v>664</v>
-      </c>
-      <c r="H15" s="23"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="13">
-        <v>468</v>
-      </c>
-      <c r="L15" s="15">
-        <v>468</v>
-      </c>
-      <c r="M15" s="11">
-        <v>479</v>
-      </c>
-      <c r="N15" s="7">
-        <v>491</v>
-      </c>
-      <c r="O15" s="7">
-        <v>469</v>
-      </c>
-      <c r="P15" s="8">
-        <v>469</v>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B21" s="23">
+        <v>1243</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="G21" s="24">
+        <v>1167</v>
+      </c>
+      <c r="H21" s="7"/>
+      <c r="I21" s="42">
+        <f>(G21-H21)/G21</f>
+        <v>1</v>
+      </c>
+      <c r="J21" s="78">
+        <v>897</v>
+      </c>
+      <c r="K21" s="43">
+        <f>(G21-J21)/G21</f>
+        <v>0.23136246786632392</v>
+      </c>
+      <c r="L21" s="25">
+        <v>1139</v>
+      </c>
+      <c r="M21" s="49"/>
+      <c r="N21" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O21" s="78">
+        <v>905</v>
+      </c>
+      <c r="P21" s="8">
+        <f t="shared" si="2"/>
+        <v>0.2054433713784021</v>
+      </c>
+      <c r="Q21" s="13">
+        <v>881</v>
+      </c>
+      <c r="R21" s="15">
+        <v>879</v>
+      </c>
+      <c r="S21" s="11">
+        <v>1020</v>
+      </c>
+      <c r="T21" s="35">
+        <v>1081</v>
+      </c>
+      <c r="U21" s="35">
+        <v>964</v>
+      </c>
+      <c r="V21" s="8">
+        <v>947</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="23">
-        <v>628</v>
-      </c>
-      <c r="F16" s="24">
-        <v>571</v>
-      </c>
-      <c r="G16" s="25">
-        <v>586</v>
-      </c>
-      <c r="H16" s="23"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="13">
-        <v>446</v>
-      </c>
-      <c r="L16" s="15">
-        <v>446</v>
-      </c>
-      <c r="M16" s="11">
-        <v>495</v>
-      </c>
-      <c r="N16" s="35">
-        <v>482</v>
-      </c>
-      <c r="O16" s="35">
-        <v>482</v>
-      </c>
-      <c r="P16" s="8">
-        <v>468</v>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B22" s="23">
+        <v>1260</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="G22" s="24">
+        <v>1207</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="I22" s="42">
+        <f>(G22-H22)/G22</f>
+        <v>1</v>
+      </c>
+      <c r="J22" s="78">
+        <v>973</v>
+      </c>
+      <c r="K22" s="43">
+        <f>(G22-J22)/G22</f>
+        <v>0.19386909693454846</v>
+      </c>
+      <c r="L22" s="25">
+        <v>1179</v>
+      </c>
+      <c r="M22" s="49"/>
+      <c r="N22" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O22" s="78">
+        <v>970</v>
+      </c>
+      <c r="P22" s="8">
+        <f t="shared" si="2"/>
+        <v>0.17726887192536048</v>
+      </c>
+      <c r="Q22" s="13">
+        <v>894</v>
+      </c>
+      <c r="R22" s="15">
+        <v>894</v>
+      </c>
+      <c r="S22" s="11">
+        <v>1030</v>
+      </c>
+      <c r="T22" s="35">
+        <v>1122</v>
+      </c>
+      <c r="U22" s="35">
+        <v>970</v>
+      </c>
+      <c r="V22" s="8">
+        <v>922</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="23">
-        <v>761</v>
-      </c>
-      <c r="F17" s="24">
-        <v>731</v>
-      </c>
-      <c r="G17" s="25">
-        <v>723</v>
-      </c>
-      <c r="H17" s="23"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="13">
-        <v>466</v>
-      </c>
-      <c r="L17" s="15">
-        <v>466</v>
-      </c>
-      <c r="M17" s="11">
-        <v>553</v>
-      </c>
-      <c r="N17" s="35">
-        <v>538</v>
-      </c>
-      <c r="O17" s="35">
-        <v>533</v>
-      </c>
-      <c r="P17" s="8">
-        <v>538</v>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B23" s="23">
+        <v>1610</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="G23" s="24">
+        <v>1500</v>
+      </c>
+      <c r="H23" s="7"/>
+      <c r="I23" s="42">
+        <f>(G23-H23)/G23</f>
+        <v>1</v>
+      </c>
+      <c r="J23" s="78">
+        <v>1154</v>
+      </c>
+      <c r="K23" s="43">
+        <f>(G23-J23)/G23</f>
+        <v>0.23066666666666666</v>
+      </c>
+      <c r="L23" s="25">
+        <v>1513</v>
+      </c>
+      <c r="M23" s="49"/>
+      <c r="N23" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O23" s="78">
+        <v>1175</v>
+      </c>
+      <c r="P23" s="8">
+        <f t="shared" si="2"/>
+        <v>0.22339722405816259</v>
+      </c>
+      <c r="Q23" s="13">
+        <v>1192</v>
+      </c>
+      <c r="R23" s="15">
+        <v>1088</v>
+      </c>
+      <c r="S23" s="11">
+        <v>1180</v>
+      </c>
+      <c r="T23" s="35">
+        <v>1243</v>
+      </c>
+      <c r="U23" s="35">
+        <v>1105</v>
+      </c>
+      <c r="V23" s="8">
+        <v>1105</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="23">
-        <v>891</v>
-      </c>
-      <c r="F18" s="24">
-        <v>851</v>
-      </c>
-      <c r="G18" s="25">
-        <v>816</v>
-      </c>
-      <c r="H18" s="23"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="13">
-        <v>554</v>
-      </c>
-      <c r="L18" s="15">
-        <v>554</v>
-      </c>
-      <c r="M18" s="11">
-        <v>656</v>
-      </c>
-      <c r="N18" s="35">
-        <v>650</v>
-      </c>
-      <c r="O18" s="35">
-        <v>634</v>
-      </c>
-      <c r="P18" s="8">
-        <v>618</v>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B24" s="26">
+        <v>2011</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="G24" s="33">
+        <v>1761</v>
+      </c>
+      <c r="H24" s="46"/>
+      <c r="I24" s="42">
+        <f>(G24-H24)/G24</f>
+        <v>1</v>
+      </c>
+      <c r="J24" s="67">
+        <v>1463</v>
+      </c>
+      <c r="K24" s="43">
+        <f>(G24-J24)/G24</f>
+        <v>0.16922203293583191</v>
+      </c>
+      <c r="L24" s="34">
+        <v>1976</v>
+      </c>
+      <c r="M24" s="46"/>
+      <c r="N24" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O24" s="67">
+        <v>1328</v>
+      </c>
+      <c r="P24" s="10">
+        <f t="shared" si="2"/>
+        <v>0.32793522267206476</v>
+      </c>
+      <c r="Q24" s="16">
+        <v>1276</v>
+      </c>
+      <c r="R24" s="18">
+        <v>1196</v>
+      </c>
+      <c r="S24" s="12">
+        <v>1538</v>
+      </c>
+      <c r="T24" s="9">
+        <v>1615</v>
+      </c>
+      <c r="U24" s="9">
+        <v>1404</v>
+      </c>
+      <c r="V24" s="10">
+        <v>1384</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="23">
-        <v>815</v>
-      </c>
-      <c r="F19" s="24">
-        <v>762</v>
-      </c>
-      <c r="G19" s="25">
-        <v>784</v>
-      </c>
-      <c r="H19" s="23"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="13">
-        <v>514</v>
-      </c>
-      <c r="L19" s="15">
-        <v>514</v>
-      </c>
-      <c r="M19" s="11">
-        <v>650</v>
-      </c>
-      <c r="N19" s="35">
-        <v>662</v>
-      </c>
-      <c r="O19" s="35">
-        <v>625</v>
-      </c>
-      <c r="P19" s="8">
-        <v>625</v>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A25" s="12"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="58">
+        <f>AVERAGE(F5:F24)</f>
+        <v>1</v>
+      </c>
+      <c r="G25" s="47"/>
+      <c r="H25" s="57"/>
+      <c r="I25" s="57">
+        <f>AVERAGE(I5:I24)</f>
+        <v>1</v>
+      </c>
+      <c r="J25" s="57"/>
+      <c r="K25" s="58">
+        <f>AVERAGE(K5:K24)</f>
+        <v>0.18456082368468371</v>
+      </c>
+      <c r="L25" s="47"/>
+      <c r="M25" s="57"/>
+      <c r="N25" s="57">
+        <f>AVERAGE(N5:N24)</f>
+        <v>1</v>
+      </c>
+      <c r="O25" s="57"/>
+      <c r="P25" s="58">
+        <f>AVERAGE(P5:P24)</f>
+        <v>0.19485870633120025</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="23">
-        <v>960</v>
-      </c>
-      <c r="F20" s="24">
-        <v>826</v>
-      </c>
-      <c r="G20" s="25">
-        <v>879</v>
-      </c>
-      <c r="H20" s="23"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="13">
-        <v>608</v>
-      </c>
-      <c r="L20" s="15">
-        <v>608</v>
-      </c>
-      <c r="M20" s="11">
-        <v>762</v>
-      </c>
-      <c r="N20" s="35">
-        <v>785</v>
-      </c>
-      <c r="O20" s="35">
-        <v>717</v>
-      </c>
-      <c r="P20" s="8">
-        <v>730</v>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="23">
-        <v>1243</v>
-      </c>
-      <c r="F21" s="24">
-        <v>1167</v>
-      </c>
-      <c r="G21" s="25">
-        <v>1139</v>
-      </c>
-      <c r="H21" s="23"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="13">
-        <v>881</v>
-      </c>
-      <c r="L21" s="15">
-        <v>879</v>
-      </c>
-      <c r="M21" s="11">
-        <v>1020</v>
-      </c>
-      <c r="N21" s="35">
-        <v>1081</v>
-      </c>
-      <c r="O21" s="35">
-        <v>964</v>
-      </c>
-      <c r="P21" s="8">
-        <v>947</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="B22" s="23"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="23">
-        <v>1260</v>
-      </c>
-      <c r="F22" s="24">
-        <v>1207</v>
-      </c>
-      <c r="G22" s="25">
-        <v>1179</v>
-      </c>
-      <c r="H22" s="23"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="13">
-        <v>894</v>
-      </c>
-      <c r="L22" s="15">
-        <v>894</v>
-      </c>
-      <c r="M22" s="11">
-        <v>1030</v>
-      </c>
-      <c r="N22" s="35">
-        <v>1122</v>
-      </c>
-      <c r="O22" s="35">
-        <v>970</v>
-      </c>
-      <c r="P22" s="8">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="23">
-        <v>1610</v>
-      </c>
-      <c r="F23" s="24">
-        <v>1500</v>
-      </c>
-      <c r="G23" s="25">
-        <v>1513</v>
-      </c>
-      <c r="H23" s="23"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="13">
-        <v>1192</v>
-      </c>
-      <c r="L23" s="15">
-        <v>1088</v>
-      </c>
-      <c r="M23" s="11">
-        <v>1180</v>
-      </c>
-      <c r="N23" s="35">
-        <v>1243</v>
-      </c>
-      <c r="O23" s="35">
-        <v>1105</v>
-      </c>
-      <c r="P23" s="8">
-        <v>1105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="B24" s="26"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="26">
-        <v>2011</v>
-      </c>
-      <c r="F24" s="33">
-        <v>1761</v>
-      </c>
-      <c r="G24" s="34">
-        <v>1976</v>
-      </c>
-      <c r="H24" s="26"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="16">
-        <v>1276</v>
-      </c>
-      <c r="L24" s="18">
-        <v>1196</v>
-      </c>
-      <c r="M24" s="12">
-        <v>1538</v>
-      </c>
-      <c r="N24" s="9">
-        <v>1615</v>
-      </c>
-      <c r="O24" s="9">
-        <v>1404</v>
-      </c>
-      <c r="P24" s="10">
-        <v>1384</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
         <v>152</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:P3"/>
+  <mergeCells count="7">
+    <mergeCell ref="S3:V3"/>
+    <mergeCell ref="B3:P3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="L4:P4"/>
+    <mergeCell ref="Q3:R3"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H3:J3"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed minor bug ignoring the precedence rule for Y-jobs
</commit_message>
<xml_diff>
--- a/data/Benchmarks/MKS.xlsx
+++ b/data/Benchmarks/MKS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\MSTS_FJSP\data\Benchmarks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BC2E9A-9B1E-489F-BAE2-78238E35F964}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73035459-4C96-4A42-9A21-90C003774406}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{87D6751E-06B1-440E-A7B4-B38AD42E9B96}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{87D6751E-06B1-440E-A7B4-B38AD42E9B96}"/>
   </bookViews>
   <sheets>
     <sheet name="Birgin Test Cases" sheetId="1" r:id="rId1"/>
@@ -959,13 +959,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -980,7 +981,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2387,7 +2387,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>295</c:v>
+                  <c:v>284</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>321</c:v>
@@ -5141,8 +5141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42C717E4-2E19-4E10-82CD-C66DD0E858F2}">
   <dimension ref="A1:Y61"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:P25"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5156,77 +5156,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="75" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="73"/>
-      <c r="P3" s="72"/>
-      <c r="Q3" s="71" t="s">
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
+      <c r="O3" s="72"/>
+      <c r="P3" s="73"/>
+      <c r="Q3" s="74" t="s">
         <v>177</v>
       </c>
-      <c r="R3" s="72"/>
-      <c r="S3" s="73" t="s">
+      <c r="R3" s="73"/>
+      <c r="S3" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="T3" s="72"/>
-      <c r="U3" s="71" t="s">
+      <c r="T3" s="73"/>
+      <c r="U3" s="74" t="s">
         <v>172</v>
       </c>
-      <c r="V3" s="72"/>
+      <c r="V3" s="73"/>
       <c r="W3" s="6"/>
       <c r="X3" s="7"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="71" t="s">
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="72"/>
-      <c r="L4" s="71" t="s">
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="73"/>
-      <c r="N4" s="73"/>
-      <c r="O4" s="73"/>
-      <c r="P4" s="72"/>
+      <c r="M4" s="72"/>
+      <c r="N4" s="72"/>
+      <c r="O4" s="72"/>
+      <c r="P4" s="73"/>
       <c r="Q4" s="3" t="s">
         <v>5</v>
       </c>
@@ -6776,61 +6776,61 @@
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
-      <c r="B27" s="71" t="s">
+      <c r="B27" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="73"/>
-      <c r="D27" s="73"/>
-      <c r="E27" s="73"/>
-      <c r="F27" s="73"/>
-      <c r="G27" s="73"/>
-      <c r="H27" s="73"/>
-      <c r="I27" s="73"/>
-      <c r="J27" s="73"/>
-      <c r="K27" s="73"/>
-      <c r="L27" s="73"/>
-      <c r="M27" s="73"/>
-      <c r="N27" s="73"/>
-      <c r="O27" s="73"/>
-      <c r="P27" s="72"/>
-      <c r="Q27" s="71" t="s">
+      <c r="C27" s="72"/>
+      <c r="D27" s="72"/>
+      <c r="E27" s="72"/>
+      <c r="F27" s="72"/>
+      <c r="G27" s="72"/>
+      <c r="H27" s="72"/>
+      <c r="I27" s="72"/>
+      <c r="J27" s="72"/>
+      <c r="K27" s="72"/>
+      <c r="L27" s="72"/>
+      <c r="M27" s="72"/>
+      <c r="N27" s="72"/>
+      <c r="O27" s="72"/>
+      <c r="P27" s="73"/>
+      <c r="Q27" s="74" t="s">
         <v>177</v>
       </c>
-      <c r="R27" s="72"/>
-      <c r="S27" s="73" t="s">
+      <c r="R27" s="73"/>
+      <c r="S27" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="T27" s="72"/>
-      <c r="U27" s="71" t="s">
+      <c r="T27" s="73"/>
+      <c r="U27" s="74" t="s">
         <v>172</v>
       </c>
-      <c r="V27" s="72"/>
+      <c r="V27" s="73"/>
       <c r="W27" s="11"/>
       <c r="X27" s="7"/>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
-      <c r="B28" s="71" t="s">
+      <c r="B28" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="C28" s="73"/>
-      <c r="D28" s="73"/>
-      <c r="E28" s="73"/>
-      <c r="F28" s="72"/>
-      <c r="G28" s="71" t="s">
+      <c r="C28" s="72"/>
+      <c r="D28" s="72"/>
+      <c r="E28" s="72"/>
+      <c r="F28" s="73"/>
+      <c r="G28" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="H28" s="73"/>
-      <c r="I28" s="73"/>
-      <c r="J28" s="73"/>
-      <c r="K28" s="72"/>
-      <c r="L28" s="71" t="s">
+      <c r="H28" s="72"/>
+      <c r="I28" s="72"/>
+      <c r="J28" s="72"/>
+      <c r="K28" s="73"/>
+      <c r="L28" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="M28" s="73"/>
-      <c r="N28" s="73"/>
-      <c r="O28" s="73"/>
-      <c r="P28" s="72"/>
+      <c r="M28" s="72"/>
+      <c r="N28" s="72"/>
+      <c r="O28" s="72"/>
+      <c r="P28" s="73"/>
       <c r="Q28" s="3" t="s">
         <v>5</v>
       </c>
@@ -6885,11 +6885,11 @@
         <v>6.8627450980392163E-2</v>
       </c>
       <c r="J29" s="69">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="K29">
         <f>(G29-J29)/G29</f>
-        <v>0.42156862745098039</v>
+        <v>0.44313725490196076</v>
       </c>
       <c r="L29" s="41">
         <v>580</v>
@@ -8970,7 +8970,7 @@
       <c r="J59" s="9"/>
       <c r="K59" s="43">
         <f>AVERAGE(K29:K58)</f>
-        <v>0.33593274192902955</v>
+        <v>0.33665169617739554</v>
       </c>
       <c r="L59" s="12"/>
       <c r="M59" s="9"/>
@@ -9000,21 +9000,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="B3:P3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="L4:P4"/>
+    <mergeCell ref="B27:P27"/>
+    <mergeCell ref="Q27:R27"/>
     <mergeCell ref="S27:T27"/>
     <mergeCell ref="U27:V27"/>
     <mergeCell ref="B28:F28"/>
     <mergeCell ref="G28:K28"/>
     <mergeCell ref="L28:P28"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="G4:K4"/>
-    <mergeCell ref="L4:P4"/>
-    <mergeCell ref="B27:P27"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="B3:P3"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9034,37 +9034,37 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="75" t="s">
         <v>153</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="71" t="s">
+      <c r="C3" s="72"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="71" t="s">
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="74" t="s">
         <v>121</v>
       </c>
-      <c r="I3" s="73"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="71" t="s">
+      <c r="I3" s="72"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="74" t="s">
         <v>154</v>
       </c>
-      <c r="L3" s="72"/>
+      <c r="L3" s="73"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
@@ -9419,7 +9419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{849930BA-C1CC-4AFE-B573-763F33389D3C}">
   <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
@@ -9429,69 +9429,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="75" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="73"/>
-      <c r="P3" s="72"/>
-      <c r="Q3" s="71" t="s">
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
+      <c r="O3" s="72"/>
+      <c r="P3" s="73"/>
+      <c r="Q3" s="74" t="s">
         <v>145</v>
       </c>
-      <c r="R3" s="72"/>
-      <c r="S3" s="75" t="s">
+      <c r="R3" s="73"/>
+      <c r="S3" s="76" t="s">
         <v>151</v>
       </c>
-      <c r="T3" s="76"/>
-      <c r="U3" s="76"/>
-      <c r="V3" s="77"/>
+      <c r="T3" s="77"/>
+      <c r="U3" s="77"/>
+      <c r="V3" s="78"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="71" t="s">
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="72"/>
-      <c r="L4" s="71" t="s">
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="73"/>
-      <c r="N4" s="73"/>
-      <c r="O4" s="73"/>
-      <c r="P4" s="72"/>
+      <c r="M4" s="72"/>
+      <c r="N4" s="72"/>
+      <c r="O4" s="72"/>
+      <c r="P4" s="73"/>
       <c r="Q4" s="3" t="s">
         <v>143</v>
       </c>
@@ -9530,14 +9530,14 @@
       </c>
       <c r="H5" s="42"/>
       <c r="I5" s="42">
-        <f>(G5-H5)/G5</f>
+        <f t="shared" ref="I5:I24" si="0">(G5-H5)/G5</f>
         <v>1</v>
       </c>
       <c r="J5" s="69">
         <v>66</v>
       </c>
       <c r="K5" s="43">
-        <f>(G5-J5)/G5</f>
+        <f t="shared" ref="K5:K24" si="1">(G5-J5)/G5</f>
         <v>0.27472527472527475</v>
       </c>
       <c r="L5" s="25">
@@ -9585,7 +9585,7 @@
       <c r="D6" s="49"/>
       <c r="E6" s="49"/>
       <c r="F6" s="8">
-        <f t="shared" ref="F6:F18" si="0">(B6-C6)/B6</f>
+        <f t="shared" ref="F6:F18" si="2">(B6-C6)/B6</f>
         <v>1</v>
       </c>
       <c r="G6" s="24">
@@ -9593,14 +9593,14 @@
       </c>
       <c r="H6" s="49"/>
       <c r="I6" s="42">
-        <f>(G6-H6)/G6</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J6" s="49">
         <v>107</v>
       </c>
       <c r="K6" s="43">
-        <f>(G6-J6)/G6</f>
+        <f t="shared" si="1"/>
         <v>0.1640625</v>
       </c>
       <c r="L6" s="25">
@@ -9608,14 +9608,14 @@
       </c>
       <c r="M6" s="49"/>
       <c r="N6" s="7">
-        <f t="shared" ref="N6:N24" si="1">(L6-M6)/L6</f>
+        <f t="shared" ref="N6:N24" si="3">(L6-M6)/L6</f>
         <v>1</v>
       </c>
       <c r="O6" s="49">
         <v>107</v>
       </c>
       <c r="P6" s="8">
-        <f t="shared" ref="P6:P24" si="2">(L6-O6)/L6</f>
+        <f t="shared" ref="P6:P24" si="4">(L6-O6)/L6</f>
         <v>0.1640625</v>
       </c>
       <c r="Q6" s="13">
@@ -9648,22 +9648,22 @@
       <c r="D7" s="51"/>
       <c r="E7" s="51"/>
       <c r="F7" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G7" s="24">
+        <v>298</v>
+      </c>
+      <c r="H7" s="49"/>
+      <c r="I7" s="42">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G7" s="24">
-        <v>298</v>
-      </c>
-      <c r="H7" s="49"/>
-      <c r="I7" s="42">
-        <f>(G7-H7)/G7</f>
-        <v>1</v>
-      </c>
-      <c r="J7" s="78">
+      <c r="J7" s="71">
         <v>236</v>
       </c>
       <c r="K7" s="43">
-        <f>(G7-J7)/G7</f>
+        <f t="shared" si="1"/>
         <v>0.20805369127516779</v>
       </c>
       <c r="L7" s="25">
@@ -9671,14 +9671,14 @@
       </c>
       <c r="M7" s="49"/>
       <c r="N7" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O7" s="49">
         <v>221</v>
       </c>
       <c r="P7" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.25838926174496646</v>
       </c>
       <c r="Q7" s="13">
@@ -9711,22 +9711,22 @@
       <c r="D8" s="65"/>
       <c r="E8" s="65"/>
       <c r="F8" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G8" s="24">
+        <v>396</v>
+      </c>
+      <c r="H8" s="49"/>
+      <c r="I8" s="42">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G8" s="24">
-        <v>396</v>
-      </c>
-      <c r="H8" s="49"/>
-      <c r="I8" s="42">
-        <f>(G8-H8)/G8</f>
-        <v>1</v>
-      </c>
       <c r="J8" s="49">
         <v>355</v>
       </c>
       <c r="K8" s="43">
-        <f>(G8-J8)/G8</f>
+        <f t="shared" si="1"/>
         <v>0.10353535353535354</v>
       </c>
       <c r="L8" s="25">
@@ -9734,14 +9734,14 @@
       </c>
       <c r="M8" s="49"/>
       <c r="N8" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O8" s="49">
         <v>355</v>
       </c>
       <c r="P8" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.10353535353535354</v>
       </c>
       <c r="Q8" s="13">
@@ -9774,22 +9774,22 @@
       <c r="D9" s="64"/>
       <c r="E9" s="64"/>
       <c r="F9" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G9" s="21">
+        <v>119</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="42">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G9" s="21">
-        <v>119</v>
-      </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="42">
-        <f>(G9-H9)/G9</f>
-        <v>1</v>
-      </c>
       <c r="J9" s="49">
         <v>119</v>
       </c>
       <c r="K9" s="43">
-        <f>(G9-J9)/G9</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L9" s="22">
@@ -9797,14 +9797,14 @@
       </c>
       <c r="M9" s="7"/>
       <c r="N9" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O9" s="65">
         <v>119</v>
       </c>
       <c r="P9" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q9" s="13">
@@ -9837,22 +9837,22 @@
       <c r="D10" s="64"/>
       <c r="E10" s="64"/>
       <c r="F10" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G10" s="24">
+        <v>360</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="42">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G10" s="24">
-        <v>360</v>
-      </c>
-      <c r="H10" s="7"/>
-      <c r="I10" s="42">
-        <f>(G10-H10)/G10</f>
-        <v>1</v>
-      </c>
       <c r="J10" s="49">
         <v>320</v>
       </c>
       <c r="K10" s="43">
-        <f>(G10-J10)/G10</f>
+        <f t="shared" si="1"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="L10" s="25">
@@ -9860,14 +9860,14 @@
       </c>
       <c r="M10" s="7"/>
       <c r="N10" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O10" s="65">
         <v>320</v>
       </c>
       <c r="P10" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="Q10" s="13">
@@ -9900,22 +9900,22 @@
       <c r="D11" s="64"/>
       <c r="E11" s="64"/>
       <c r="F11" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G11" s="21">
+        <v>397</v>
+      </c>
+      <c r="H11" s="7"/>
+      <c r="I11" s="42">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G11" s="21">
-        <v>397</v>
-      </c>
-      <c r="H11" s="7"/>
-      <c r="I11" s="42">
-        <f>(G11-H11)/G11</f>
-        <v>1</v>
-      </c>
       <c r="J11" s="49">
         <v>397</v>
       </c>
       <c r="K11" s="43">
-        <f>(G11-J11)/G11</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L11" s="22">
@@ -9923,14 +9923,14 @@
       </c>
       <c r="M11" s="7"/>
       <c r="N11" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O11" s="65">
         <v>397</v>
       </c>
       <c r="P11" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q11" s="13">
@@ -9963,22 +9963,22 @@
       <c r="D12" s="64"/>
       <c r="E12" s="64"/>
       <c r="F12" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G12" s="24">
+        <v>325</v>
+      </c>
+      <c r="H12" s="49"/>
+      <c r="I12" s="42">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G12" s="24">
-        <v>325</v>
-      </c>
-      <c r="H12" s="49"/>
-      <c r="I12" s="42">
-        <f>(G12-H12)/G12</f>
-        <v>1</v>
-      </c>
       <c r="J12" s="49">
         <v>253</v>
       </c>
       <c r="K12" s="43">
-        <f>(G12-J12)/G12</f>
+        <f t="shared" si="1"/>
         <v>0.22153846153846155</v>
       </c>
       <c r="L12" s="25">
@@ -9986,14 +9986,14 @@
       </c>
       <c r="M12" s="49"/>
       <c r="N12" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O12" s="49">
         <v>253</v>
       </c>
       <c r="P12" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.22153846153846155</v>
       </c>
       <c r="Q12" s="13">
@@ -10026,22 +10026,22 @@
       <c r="D13" s="65"/>
       <c r="E13" s="65"/>
       <c r="F13" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G13" s="24">
+        <v>290</v>
+      </c>
+      <c r="H13" s="49"/>
+      <c r="I13" s="42">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G13" s="24">
-        <v>290</v>
-      </c>
-      <c r="H13" s="49"/>
-      <c r="I13" s="42">
-        <f>(G13-H13)/G13</f>
-        <v>1</v>
-      </c>
-      <c r="J13" s="78">
+      <c r="J13" s="71">
         <v>220</v>
       </c>
       <c r="K13" s="43">
-        <f>(G13-J13)/G13</f>
+        <f t="shared" si="1"/>
         <v>0.2413793103448276</v>
       </c>
       <c r="L13" s="25">
@@ -10049,14 +10049,14 @@
       </c>
       <c r="M13" s="49"/>
       <c r="N13" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O13" s="49">
         <v>210</v>
       </c>
       <c r="P13" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.1828793774319066</v>
       </c>
       <c r="Q13" s="13">
@@ -10089,22 +10089,22 @@
       <c r="D14" s="64"/>
       <c r="E14" s="64"/>
       <c r="F14" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G14" s="36">
+        <v>516</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="42">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G14" s="36">
-        <v>516</v>
-      </c>
-      <c r="H14" s="7"/>
-      <c r="I14" s="42">
-        <f>(G14-H14)/G14</f>
-        <v>1</v>
-      </c>
       <c r="J14" s="49">
         <v>516</v>
       </c>
       <c r="K14" s="43">
-        <f>(G14-J14)/G14</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L14" s="37">
@@ -10112,14 +10112,14 @@
       </c>
       <c r="M14" s="7"/>
       <c r="N14" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O14" s="65">
         <v>516</v>
       </c>
       <c r="P14" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q14" s="16">
@@ -10152,22 +10152,22 @@
       <c r="D15" s="65"/>
       <c r="E15" s="65"/>
       <c r="F15" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G15" s="24">
+        <v>664</v>
+      </c>
+      <c r="H15" s="49"/>
+      <c r="I15" s="42">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G15" s="24">
-        <v>664</v>
-      </c>
-      <c r="H15" s="49"/>
-      <c r="I15" s="42">
-        <f>(G15-H15)/G15</f>
-        <v>1</v>
-      </c>
-      <c r="J15" s="78">
+      <c r="J15" s="71">
         <v>479</v>
       </c>
       <c r="K15" s="43">
-        <f>(G15-J15)/G15</f>
+        <f t="shared" si="1"/>
         <v>0.27861445783132532</v>
       </c>
       <c r="L15" s="25">
@@ -10175,14 +10175,14 @@
       </c>
       <c r="M15" s="49"/>
       <c r="N15" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="O15" s="78">
+      <c r="O15" s="71">
         <v>495</v>
       </c>
       <c r="P15" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.25451807228915663</v>
       </c>
       <c r="Q15" s="13">
@@ -10215,22 +10215,22 @@
       <c r="D16" s="66"/>
       <c r="E16" s="66"/>
       <c r="F16" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G16" s="24">
+        <v>571</v>
+      </c>
+      <c r="H16" s="51"/>
+      <c r="I16" s="42">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G16" s="24">
-        <v>571</v>
-      </c>
-      <c r="H16" s="51"/>
-      <c r="I16" s="42">
-        <f>(G16-H16)/G16</f>
-        <v>1</v>
-      </c>
-      <c r="J16" s="78">
+      <c r="J16" s="71">
         <v>459</v>
       </c>
       <c r="K16" s="43">
-        <f>(G16-J16)/G16</f>
+        <f t="shared" si="1"/>
         <v>0.19614711033274956</v>
       </c>
       <c r="L16" s="25">
@@ -10238,14 +10238,14 @@
       </c>
       <c r="M16" s="7"/>
       <c r="N16" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O16" s="68">
         <v>466</v>
       </c>
       <c r="P16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.20477815699658702</v>
       </c>
       <c r="Q16" s="13">
@@ -10278,22 +10278,22 @@
       <c r="D17" s="66"/>
       <c r="E17" s="66"/>
       <c r="F17" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G17" s="24">
+        <v>731</v>
+      </c>
+      <c r="H17" s="51"/>
+      <c r="I17" s="42">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G17" s="24">
-        <v>731</v>
-      </c>
-      <c r="H17" s="51"/>
-      <c r="I17" s="42">
-        <f>(G17-H17)/G17</f>
-        <v>1</v>
-      </c>
-      <c r="J17" s="78">
+      <c r="J17" s="71">
         <v>473</v>
       </c>
       <c r="K17" s="43">
-        <f>(G17-J17)/G17</f>
+        <f t="shared" si="1"/>
         <v>0.35294117647058826</v>
       </c>
       <c r="L17" s="25">
@@ -10301,14 +10301,14 @@
       </c>
       <c r="M17" s="49"/>
       <c r="N17" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="O17" s="78">
+      <c r="O17" s="71">
         <v>479</v>
       </c>
       <c r="P17" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.33748271092669435</v>
       </c>
       <c r="Q17" s="13">
@@ -10341,22 +10341,22 @@
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G18" s="24">
+        <v>851</v>
+      </c>
+      <c r="H18" s="51"/>
+      <c r="I18" s="42">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G18" s="24">
-        <v>851</v>
-      </c>
-      <c r="H18" s="51"/>
-      <c r="I18" s="42">
-        <f>(G18-H18)/G18</f>
-        <v>1</v>
-      </c>
-      <c r="J18" s="78">
+      <c r="J18" s="71">
         <v>572</v>
       </c>
       <c r="K18" s="43">
-        <f>(G18-J18)/G18</f>
+        <f t="shared" si="1"/>
         <v>0.32784958871915393</v>
       </c>
       <c r="L18" s="25">
@@ -10364,14 +10364,14 @@
       </c>
       <c r="M18" s="51"/>
       <c r="N18" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="O18" s="78">
+      <c r="O18" s="71">
         <v>567</v>
       </c>
       <c r="P18" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.30514705882352944</v>
       </c>
       <c r="Q18" s="13">
@@ -10411,14 +10411,14 @@
       </c>
       <c r="H19" s="7"/>
       <c r="I19" s="42">
-        <f>(G19-H19)/G19</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J19" s="78">
+      <c r="J19" s="71">
         <v>584</v>
       </c>
       <c r="K19" s="43">
-        <f>(G19-J19)/G19</f>
+        <f t="shared" si="1"/>
         <v>0.23359580052493439</v>
       </c>
       <c r="L19" s="25">
@@ -10426,14 +10426,14 @@
       </c>
       <c r="M19" s="49"/>
       <c r="N19" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="O19" s="78">
+      <c r="O19" s="71">
         <v>561</v>
       </c>
       <c r="P19" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.28443877551020408</v>
       </c>
       <c r="Q19" s="13">
@@ -10473,14 +10473,14 @@
       </c>
       <c r="H20" s="49"/>
       <c r="I20" s="42">
-        <f>(G20-H20)/G20</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J20" s="78">
+      <c r="J20" s="71">
         <v>700</v>
       </c>
       <c r="K20" s="43">
-        <f>(G20-J20)/G20</f>
+        <f t="shared" si="1"/>
         <v>0.15254237288135594</v>
       </c>
       <c r="L20" s="25">
@@ -10488,14 +10488,14 @@
       </c>
       <c r="M20" s="49"/>
       <c r="N20" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="O20" s="78">
+      <c r="O20" s="71">
         <v>650</v>
       </c>
       <c r="P20" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.26052332195676908</v>
       </c>
       <c r="Q20" s="13">
@@ -10535,14 +10535,14 @@
       </c>
       <c r="H21" s="7"/>
       <c r="I21" s="42">
-        <f>(G21-H21)/G21</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J21" s="78">
+      <c r="J21" s="71">
         <v>897</v>
       </c>
       <c r="K21" s="43">
-        <f>(G21-J21)/G21</f>
+        <f t="shared" si="1"/>
         <v>0.23136246786632392</v>
       </c>
       <c r="L21" s="25">
@@ -10550,14 +10550,14 @@
       </c>
       <c r="M21" s="49"/>
       <c r="N21" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="O21" s="78">
+      <c r="O21" s="71">
         <v>905</v>
       </c>
       <c r="P21" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.2054433713784021</v>
       </c>
       <c r="Q21" s="13">
@@ -10597,14 +10597,14 @@
       </c>
       <c r="H22" s="7"/>
       <c r="I22" s="42">
-        <f>(G22-H22)/G22</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J22" s="78">
+      <c r="J22" s="71">
         <v>973</v>
       </c>
       <c r="K22" s="43">
-        <f>(G22-J22)/G22</f>
+        <f t="shared" si="1"/>
         <v>0.19386909693454846</v>
       </c>
       <c r="L22" s="25">
@@ -10612,14 +10612,14 @@
       </c>
       <c r="M22" s="49"/>
       <c r="N22" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="O22" s="78">
+      <c r="O22" s="71">
         <v>970</v>
       </c>
       <c r="P22" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.17726887192536048</v>
       </c>
       <c r="Q22" s="13">
@@ -10659,14 +10659,14 @@
       </c>
       <c r="H23" s="7"/>
       <c r="I23" s="42">
-        <f>(G23-H23)/G23</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J23" s="78">
+      <c r="J23" s="71">
         <v>1154</v>
       </c>
       <c r="K23" s="43">
-        <f>(G23-J23)/G23</f>
+        <f t="shared" si="1"/>
         <v>0.23066666666666666</v>
       </c>
       <c r="L23" s="25">
@@ -10674,14 +10674,14 @@
       </c>
       <c r="M23" s="49"/>
       <c r="N23" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="O23" s="78">
+      <c r="O23" s="71">
         <v>1175</v>
       </c>
       <c r="P23" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.22339722405816259</v>
       </c>
       <c r="Q23" s="13">
@@ -10721,14 +10721,14 @@
       </c>
       <c r="H24" s="46"/>
       <c r="I24" s="42">
-        <f>(G24-H24)/G24</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J24" s="67">
         <v>1463</v>
       </c>
       <c r="K24" s="43">
-        <f>(G24-J24)/G24</f>
+        <f t="shared" si="1"/>
         <v>0.16922203293583191</v>
       </c>
       <c r="L24" s="34">
@@ -10736,14 +10736,14 @@
       </c>
       <c r="M24" s="46"/>
       <c r="N24" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O24" s="67">
         <v>1328</v>
       </c>
       <c r="P24" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.32793522267206476</v>
       </c>
       <c r="Q24" s="16">
@@ -10810,13 +10810,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A1:G1"/>
     <mergeCell ref="S3:V3"/>
     <mergeCell ref="B3:P3"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="G4:K4"/>
     <mergeCell ref="L4:P4"/>
     <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>